<commit_message>
.json files, .xls content editado
</commit_message>
<xml_diff>
--- a/03_design/architecture-copy.xlsx
+++ b/03_design/architecture-copy.xlsx
@@ -4,21 +4,23 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="15255" windowHeight="12285" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="15255" windowHeight="12285"/>
   </bookViews>
   <sheets>
     <sheet name="main page" sheetId="1" r:id="rId1"/>
     <sheet name="project page" sheetId="2" r:id="rId2"/>
     <sheet name="folder architecure" sheetId="4" r:id="rId3"/>
-    <sheet name="filters" sheetId="3" r:id="rId4"/>
-    <sheet name="schools" sheetId="5" r:id="rId5"/>
+    <sheet name="filters.json" sheetId="3" r:id="rId4"/>
+    <sheet name="courses.json" sheetId="5" r:id="rId5"/>
+    <sheet name="notas" sheetId="6" r:id="rId6"/>
+    <sheet name="Folha2" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="254">
   <si>
     <t>Main page</t>
   </si>
@@ -321,42 +323,6 @@
     <t>pTools</t>
   </si>
   <si>
-    <t>Photoshop;</t>
-  </si>
-  <si>
-    <t>Illustrator;</t>
-  </si>
-  <si>
-    <t>InDesign;</t>
-  </si>
-  <si>
-    <t>Flash;</t>
-  </si>
-  <si>
-    <t>Premier;</t>
-  </si>
-  <si>
-    <t>Figma;</t>
-  </si>
-  <si>
-    <t>HTML;</t>
-  </si>
-  <si>
-    <t>CSS;</t>
-  </si>
-  <si>
-    <t>JavaScript;</t>
-  </si>
-  <si>
-    <t>React;</t>
-  </si>
-  <si>
-    <t>PHP;</t>
-  </si>
-  <si>
-    <t>fields:</t>
-  </si>
-  <si>
     <t>Branding</t>
   </si>
   <si>
@@ -364,12 +330,6 @@
   </si>
   <si>
     <t>UX/UI Design / web Design</t>
-  </si>
-  <si>
-    <t>schools:</t>
-  </si>
-  <si>
-    <t>context:</t>
   </si>
   <si>
     <t>span</t>
@@ -957,9 +917,6 @@
     <t>(icone) nav-menu</t>
   </si>
   <si>
-    <t>icon</t>
-  </si>
-  <si>
     <t>kid_star</t>
   </si>
   <si>
@@ -994,13 +951,175 @@
   </si>
   <si>
     <t>person</t>
+  </si>
+  <si>
+    <t>fields</t>
+  </si>
+  <si>
+    <t>schools</t>
+  </si>
+  <si>
+    <t>context</t>
+  </si>
+  <si>
+    <t>icones</t>
+  </si>
+  <si>
+    <t>https://www.svgrepo.com/</t>
+  </si>
+  <si>
+    <t>https://fonts.google.com/icons</t>
+  </si>
+  <si>
+    <t>LinkedIn</t>
+  </si>
+  <si>
+    <t>Behance</t>
+  </si>
+  <si>
+    <t>Instagram</t>
+  </si>
+  <si>
+    <t>contact</t>
+  </si>
+  <si>
+    <t>tools</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>Figma</t>
+  </si>
+  <si>
+    <t>Flash</t>
+  </si>
+  <si>
+    <t>Illustrator</t>
+  </si>
+  <si>
+    <t>InDesign</t>
+  </si>
+  <si>
+    <t>Premier</t>
+  </si>
+  <si>
+    <t>CSS</t>
+  </si>
+  <si>
+    <t>HTML</t>
+  </si>
+  <si>
+    <t>JavaScript</t>
+  </si>
+  <si>
+    <t>PHP</t>
+  </si>
+  <si>
+    <t>React</t>
+  </si>
+  <si>
+    <t>Photoshop</t>
+  </si>
+  <si>
+    <t>local-svg</t>
+  </si>
+  <si>
+    <t>fonts-google</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>label</t>
+  </si>
+  <si>
+    <t>mariosilva/src/assets/icons/tools/adobe-flash.svg</t>
+  </si>
+  <si>
+    <t>mariosilva/src/assets/icons/tools/adobe-illustrator.svg</t>
+  </si>
+  <si>
+    <t>mariosilva/src/assets/icons/tools/adobe-indesign.svg</t>
+  </si>
+  <si>
+    <t>mariosilva/src/assets/icons/tools/adobe-photoshop.svg</t>
+  </si>
+  <si>
+    <t>mariosilva/src/assets/icons/tools/adobe-premierpro.svg</t>
+  </si>
+  <si>
+    <t>mariosilva/src/assets/icons/tools/css3.svg</t>
+  </si>
+  <si>
+    <t>mariosilva/src/assets/icons/tools/figma.svg</t>
+  </si>
+  <si>
+    <t>mariosilva/src/assets/icons/tools/html5.svg</t>
+  </si>
+  <si>
+    <t>mariosilva/src/assets/icons/tools/javascript.svg</t>
+  </si>
+  <si>
+    <t>mariosilva/src/assets/icons/tools/php.svg</t>
+  </si>
+  <si>
+    <t>mariosilva/src/assets/icons/tools/react.svg</t>
+  </si>
+  <si>
+    <t>mariosilva/src/assets/icons/contact/behance.svg</t>
+  </si>
+  <si>
+    <t>mariosilva/src/assets/icons/contact/instagram.svg</t>
+  </si>
+  <si>
+    <t>mariosilva/src/assets/icons/contact/linkedin.svg</t>
+  </si>
+  <si>
+    <t>2021 – 2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User Experience &amp; User Interface </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024 – 2025 </t>
+  </si>
+  <si>
+    <t>Flagprofessional Fullstack Web Development</t>
+  </si>
+  <si>
+    <t>351h</t>
+  </si>
+  <si>
+    <t>216h</t>
+  </si>
+  <si>
+    <t>363h</t>
+  </si>
+  <si>
+    <t>course</t>
+  </si>
+  <si>
+    <t>hours</t>
+  </si>
+  <si>
+    <t>period</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flagprofessional Graphic Designer </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1023,6 +1142,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -1162,10 +1288,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1247,9 +1377,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1307,45 +1434,74 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="5"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hiperligação" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1640,8 +1796,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G68"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33:B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1656,14 +1812,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
       <c r="G1" s="3"/>
     </row>
     <row r="2" spans="1:7" ht="37.5" customHeight="1" thickBot="1">
@@ -1677,7 +1833,7 @@
       <c r="D2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="42"/>
+      <c r="E2" s="41"/>
       <c r="F2" s="4" t="s">
         <v>4</v>
       </c>
@@ -1685,789 +1841,788 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="36" customFormat="1" ht="15.75" thickTop="1">
-      <c r="A3" s="53" t="s">
+    <row r="3" spans="1:7" s="35" customFormat="1" ht="15.75" thickTop="1">
+      <c r="A3" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="33"/>
-      <c r="C3" s="33" t="s">
+      <c r="B3" s="32"/>
+      <c r="C3" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="33"/>
-      <c r="E3" s="34" t="s">
+      <c r="D3" s="32"/>
+      <c r="E3" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="35"/>
+      <c r="G3" s="34"/>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="53"/>
+      <c r="A4" s="52"/>
       <c r="B4" s="12"/>
-      <c r="C4" s="53" t="s">
+      <c r="C4" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="53" t="s">
+      <c r="D4" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="40"/>
+      <c r="E4" s="39"/>
       <c r="F4" s="5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="53"/>
+      <c r="A5" s="52"/>
       <c r="B5" s="12"/>
-      <c r="C5" s="53"/>
-      <c r="D5" s="53"/>
-      <c r="E5" s="40"/>
+      <c r="C5" s="52"/>
+      <c r="D5" s="52"/>
+      <c r="E5" s="39"/>
       <c r="F5" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="53"/>
+      <c r="A6" s="52"/>
       <c r="B6" s="12"/>
-      <c r="C6" s="53"/>
-      <c r="D6" s="53"/>
-      <c r="E6" s="40"/>
+      <c r="C6" s="52"/>
+      <c r="D6" s="52"/>
+      <c r="E6" s="39"/>
       <c r="F6" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="53"/>
+      <c r="A7" s="52"/>
       <c r="B7" s="12"/>
-      <c r="C7" s="53"/>
-      <c r="D7" s="53"/>
-      <c r="E7" s="40"/>
+      <c r="C7" s="52"/>
+      <c r="D7" s="52"/>
+      <c r="E7" s="39"/>
       <c r="F7" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A8" s="45"/>
-      <c r="B8" s="45"/>
-      <c r="C8" s="45"/>
-      <c r="D8" s="45"/>
-      <c r="E8" s="45" t="s">
-        <v>201</v>
-      </c>
-      <c r="F8" s="45"/>
-    </row>
-    <row r="9" spans="1:7" s="36" customFormat="1" ht="15.75" thickTop="1">
-      <c r="A9" s="53" t="s">
+      <c r="A8" s="44"/>
+      <c r="B8" s="44"/>
+      <c r="C8" s="44"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="44" t="s">
+        <v>187</v>
+      </c>
+      <c r="F8" s="44"/>
+    </row>
+    <row r="9" spans="1:7" s="35" customFormat="1" ht="15.75" thickTop="1">
+      <c r="A9" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="33"/>
-      <c r="C9" s="33" t="s">
+      <c r="B9" s="32"/>
+      <c r="C9" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="33"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="34" t="s">
+      <c r="D9" s="32"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="G9" s="35"/>
+      <c r="G9" s="34"/>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="53"/>
+      <c r="A10" s="52"/>
       <c r="B10" s="12"/>
-      <c r="C10" s="53" t="s">
+      <c r="C10" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="53" t="s">
+      <c r="D10" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="40"/>
+      <c r="E10" s="39"/>
       <c r="F10" s="26" t="s">
-        <v>139</v>
+        <v>125</v>
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="53"/>
+      <c r="A11" s="52"/>
       <c r="B11" s="12"/>
-      <c r="C11" s="53"/>
-      <c r="D11" s="53"/>
-      <c r="E11" s="40"/>
+      <c r="C11" s="52"/>
+      <c r="D11" s="52"/>
+      <c r="E11" s="39"/>
       <c r="F11" s="26" t="s">
-        <v>140</v>
+        <v>126</v>
       </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="53"/>
+      <c r="A12" s="52"/>
       <c r="B12" s="12"/>
-      <c r="C12" s="53"/>
-      <c r="D12" s="53"/>
-      <c r="E12" s="40"/>
+      <c r="C12" s="52"/>
+      <c r="D12" s="52"/>
+      <c r="E12" s="39"/>
       <c r="F12" s="26" t="s">
-        <v>141</v>
+        <v>127</v>
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="53"/>
+      <c r="A13" s="52"/>
       <c r="B13" s="12"/>
-      <c r="C13" s="53"/>
-      <c r="D13" s="53"/>
-      <c r="E13" s="40"/>
+      <c r="C13" s="52"/>
+      <c r="D13" s="52"/>
+      <c r="E13" s="39"/>
       <c r="F13" s="26" t="s">
-        <v>142</v>
+        <v>128</v>
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="53"/>
+      <c r="A14" s="52"/>
       <c r="B14" s="12"/>
-      <c r="C14" s="53"/>
-      <c r="D14" s="53"/>
-      <c r="E14" s="40"/>
+      <c r="C14" s="52"/>
+      <c r="D14" s="52"/>
+      <c r="E14" s="39"/>
       <c r="F14" s="26" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="53"/>
+      <c r="A15" s="52"/>
       <c r="B15" s="12"/>
-      <c r="C15" s="53"/>
-      <c r="D15" s="53"/>
-      <c r="E15" s="40"/>
+      <c r="C15" s="52"/>
+      <c r="D15" s="52"/>
+      <c r="E15" s="39"/>
       <c r="F15" s="26" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="53"/>
+      <c r="A16" s="52"/>
       <c r="B16" s="12"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E16" s="40"/>
+      <c r="E16" s="39"/>
       <c r="F16" s="14" t="s">
-        <v>145</v>
+        <v>131</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A17" s="53"/>
+      <c r="A17" s="52"/>
       <c r="B17" s="12"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E17" s="40"/>
+      <c r="E17" s="39"/>
       <c r="F17" s="27" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" s="36" customFormat="1" ht="15.75" thickTop="1">
-      <c r="A18" s="55" t="s">
-        <v>157</v>
-      </c>
-      <c r="B18" s="54" t="s">
-        <v>156</v>
-      </c>
-      <c r="C18" s="53" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" s="35" customFormat="1" ht="15.75" thickTop="1">
+      <c r="A18" s="58" t="s">
+        <v>143</v>
+      </c>
+      <c r="B18" s="53" t="s">
+        <v>142</v>
+      </c>
+      <c r="C18" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="D18" s="54" t="s">
+      <c r="D18" s="53" t="s">
         <v>23</v>
       </c>
-      <c r="E18" s="41"/>
-      <c r="F18" s="37" t="s">
-        <v>83</v>
-      </c>
-      <c r="G18" s="35"/>
+      <c r="E18" s="40"/>
+      <c r="F18" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="G18" s="34"/>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="55"/>
-      <c r="B19" s="54"/>
-      <c r="C19" s="53"/>
-      <c r="D19" s="54"/>
-      <c r="E19" s="41"/>
+      <c r="A19" s="58"/>
+      <c r="B19" s="53"/>
+      <c r="C19" s="52"/>
+      <c r="D19" s="53"/>
+      <c r="E19" s="40"/>
       <c r="F19" s="14" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="55"/>
-      <c r="B20" s="54"/>
-      <c r="C20" s="53"/>
-      <c r="D20" s="53"/>
-      <c r="E20" s="40"/>
+      <c r="A20" s="58"/>
+      <c r="B20" s="53"/>
+      <c r="C20" s="52"/>
+      <c r="D20" s="52"/>
+      <c r="E20" s="39"/>
       <c r="F20" s="14" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="55"/>
-      <c r="B21" s="54"/>
-      <c r="C21" s="53"/>
-      <c r="D21" s="53"/>
-      <c r="E21" s="40"/>
+      <c r="A21" s="58"/>
+      <c r="B21" s="53"/>
+      <c r="C21" s="52"/>
+      <c r="D21" s="52"/>
+      <c r="E21" s="39"/>
       <c r="F21" s="14" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="55"/>
-      <c r="B22" s="54"/>
-      <c r="C22" s="53"/>
-      <c r="D22" s="53"/>
-      <c r="E22" s="40"/>
+      <c r="A22" s="58"/>
+      <c r="B22" s="53"/>
+      <c r="C22" s="52"/>
+      <c r="D22" s="52"/>
+      <c r="E22" s="39"/>
       <c r="F22" s="14" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" s="55"/>
-      <c r="B23" s="54"/>
-      <c r="C23" s="53"/>
-      <c r="D23" s="53"/>
-      <c r="E23" s="40"/>
+      <c r="A23" s="58"/>
+      <c r="B23" s="53"/>
+      <c r="C23" s="52"/>
+      <c r="D23" s="52"/>
+      <c r="E23" s="39"/>
       <c r="F23" s="14" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:7">
-      <c r="A24" s="55"/>
-      <c r="B24" s="54"/>
-      <c r="C24" s="53"/>
-      <c r="D24" s="53"/>
-      <c r="E24" s="40"/>
+      <c r="A24" s="58"/>
+      <c r="B24" s="53"/>
+      <c r="C24" s="52"/>
+      <c r="D24" s="52"/>
+      <c r="E24" s="39"/>
       <c r="F24" s="26" t="s">
-        <v>155</v>
+        <v>141</v>
       </c>
     </row>
     <row r="25" spans="1:7">
-      <c r="A25" s="55"/>
-      <c r="B25" s="54"/>
-      <c r="C25" s="53"/>
-      <c r="D25" s="53"/>
-      <c r="E25" s="40"/>
+      <c r="A25" s="58"/>
+      <c r="B25" s="53"/>
+      <c r="C25" s="52"/>
+      <c r="D25" s="52"/>
+      <c r="E25" s="39"/>
       <c r="F25" s="14" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="55"/>
-      <c r="B26" s="54"/>
-      <c r="C26" s="53"/>
-      <c r="D26" s="54" t="s">
+      <c r="A26" s="58"/>
+      <c r="B26" s="53"/>
+      <c r="C26" s="52"/>
+      <c r="D26" s="53" t="s">
         <v>30</v>
       </c>
-      <c r="E26" s="41"/>
+      <c r="E26" s="40"/>
       <c r="F26" s="14" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="27" spans="1:7">
-      <c r="A27" s="55"/>
-      <c r="B27" s="54"/>
-      <c r="C27" s="53"/>
-      <c r="D27" s="53"/>
-      <c r="E27" s="40"/>
+      <c r="A27" s="58"/>
+      <c r="B27" s="53"/>
+      <c r="C27" s="52"/>
+      <c r="D27" s="52"/>
+      <c r="E27" s="39"/>
       <c r="F27" s="14" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" s="55"/>
-      <c r="B28" s="54"/>
-      <c r="C28" s="53"/>
-      <c r="D28" s="53"/>
-      <c r="E28" s="40"/>
+      <c r="A28" s="58"/>
+      <c r="B28" s="53"/>
+      <c r="C28" s="52"/>
+      <c r="D28" s="52"/>
+      <c r="E28" s="39"/>
       <c r="F28" s="14" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="29" spans="1:7">
-      <c r="A29" s="55"/>
-      <c r="B29" s="54"/>
-      <c r="C29" s="53"/>
-      <c r="D29" s="54" t="s">
+      <c r="A29" s="58"/>
+      <c r="B29" s="53"/>
+      <c r="C29" s="52"/>
+      <c r="D29" s="53" t="s">
         <v>34</v>
       </c>
-      <c r="E29" s="41"/>
+      <c r="E29" s="40"/>
       <c r="F29" s="14" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="30" spans="1:7">
-      <c r="A30" s="55"/>
-      <c r="B30" s="54"/>
-      <c r="C30" s="53"/>
-      <c r="D30" s="53"/>
-      <c r="E30" s="40"/>
+      <c r="A30" s="58"/>
+      <c r="B30" s="53"/>
+      <c r="C30" s="52"/>
+      <c r="D30" s="52"/>
+      <c r="E30" s="39"/>
       <c r="F30" s="14" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="31" spans="1:7">
-      <c r="A31" s="55"/>
-      <c r="B31" s="54"/>
-      <c r="C31" s="53"/>
-      <c r="D31" s="53"/>
-      <c r="E31" s="40"/>
+      <c r="A31" s="58"/>
+      <c r="B31" s="53"/>
+      <c r="C31" s="52"/>
+      <c r="D31" s="52"/>
+      <c r="E31" s="39"/>
       <c r="F31" s="14" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="32" spans="1:7">
-      <c r="A32" s="55"/>
-      <c r="B32" s="54"/>
-      <c r="C32" s="53"/>
-      <c r="D32" s="53"/>
-      <c r="E32" s="40"/>
+      <c r="A32" s="58"/>
+      <c r="B32" s="53"/>
+      <c r="C32" s="52"/>
+      <c r="D32" s="52"/>
+      <c r="E32" s="39"/>
       <c r="F32" s="14" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="33" spans="1:7">
-      <c r="A33" s="55"/>
-      <c r="B33" s="59" t="s">
+      <c r="A33" s="58"/>
+      <c r="B33" s="56" t="s">
         <v>21</v>
       </c>
-      <c r="C33" s="59" t="s">
+      <c r="C33" s="56" t="s">
+        <v>169</v>
+      </c>
+      <c r="D33" s="40" t="s">
+        <v>186</v>
+      </c>
+      <c r="E33" s="39"/>
+      <c r="F33" s="40"/>
+    </row>
+    <row r="34" spans="1:7" s="29" customFormat="1">
+      <c r="A34" s="58"/>
+      <c r="B34" s="56"/>
+      <c r="C34" s="56"/>
+      <c r="D34" s="53" t="s">
+        <v>170</v>
+      </c>
+      <c r="E34" s="30" t="s">
+        <v>171</v>
+      </c>
+      <c r="F34" s="28"/>
+      <c r="G34" s="68" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" s="58"/>
+      <c r="B35" s="56"/>
+      <c r="C35" s="56"/>
+      <c r="D35" s="53"/>
+      <c r="E35" s="30" t="s">
+        <v>172</v>
+      </c>
+      <c r="F35" s="50" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" s="58"/>
+      <c r="B36" s="56"/>
+      <c r="C36" s="56"/>
+      <c r="D36" s="53"/>
+      <c r="E36" s="30" t="s">
+        <v>174</v>
+      </c>
+      <c r="F36" s="40" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" s="58"/>
+      <c r="B37" s="56"/>
+      <c r="C37" s="56"/>
+      <c r="D37" s="53"/>
+      <c r="E37" s="30" t="s">
+        <v>173</v>
+      </c>
+      <c r="F37" s="11" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" s="58"/>
+      <c r="B38" s="56"/>
+      <c r="C38" s="56"/>
+      <c r="D38" s="53"/>
+      <c r="E38" s="30" t="s">
+        <v>174</v>
+      </c>
+      <c r="F38" s="40" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" s="58"/>
+      <c r="B39" s="56"/>
+      <c r="C39" s="56"/>
+      <c r="D39" s="53"/>
+      <c r="E39" s="30" t="s">
+        <v>175</v>
+      </c>
+      <c r="F39" s="42" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40" s="58"/>
+      <c r="B40" s="56"/>
+      <c r="C40" s="56"/>
+      <c r="D40" s="59"/>
+      <c r="E40" s="47" t="s">
+        <v>176</v>
+      </c>
+      <c r="F40" s="48" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" s="58"/>
+      <c r="B41" s="56"/>
+      <c r="C41" s="56"/>
+      <c r="D41" s="31"/>
+      <c r="E41" s="30"/>
+      <c r="F41" s="40" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42" s="58"/>
+      <c r="B42" s="56"/>
+      <c r="C42" s="56"/>
+      <c r="D42" s="31"/>
+      <c r="E42" s="30"/>
+      <c r="F42" s="40" t="s">
         <v>183</v>
       </c>
-      <c r="D33" s="41" t="s">
-        <v>200</v>
-      </c>
-      <c r="E33" s="40"/>
-      <c r="F33" s="41"/>
-    </row>
-    <row r="34" spans="1:7" s="30" customFormat="1">
-      <c r="A34" s="55"/>
-      <c r="B34" s="59"/>
-      <c r="C34" s="59"/>
-      <c r="D34" s="54" t="s">
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43" s="58"/>
+      <c r="B43" s="56"/>
+      <c r="C43" s="56"/>
+      <c r="D43" s="49"/>
+      <c r="E43" s="49"/>
+      <c r="F43" s="40" t="s">
         <v>184</v>
       </c>
-      <c r="E34" s="31" t="s">
-        <v>185</v>
-      </c>
-      <c r="F34" s="28"/>
-      <c r="G34" s="29" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7">
-      <c r="A35" s="55"/>
-      <c r="B35" s="59"/>
-      <c r="C35" s="59"/>
-      <c r="D35" s="54"/>
-      <c r="E35" s="31" t="s">
-        <v>186</v>
-      </c>
-      <c r="F35" s="41" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7">
-      <c r="A36" s="55"/>
-      <c r="B36" s="59"/>
-      <c r="C36" s="59"/>
-      <c r="D36" s="54"/>
-      <c r="E36" s="31" t="s">
-        <v>188</v>
-      </c>
-      <c r="F36" s="41" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7">
-      <c r="A37" s="55"/>
-      <c r="B37" s="59"/>
-      <c r="C37" s="59"/>
-      <c r="D37" s="54"/>
-      <c r="E37" s="31" t="s">
-        <v>187</v>
-      </c>
-      <c r="F37" s="11" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7">
-      <c r="A38" s="55"/>
-      <c r="B38" s="59"/>
-      <c r="C38" s="59"/>
-      <c r="D38" s="54"/>
-      <c r="E38" s="31" t="s">
-        <v>188</v>
-      </c>
-      <c r="F38" s="41" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7">
-      <c r="A39" s="55"/>
-      <c r="B39" s="59"/>
-      <c r="C39" s="59"/>
-      <c r="D39" s="54"/>
-      <c r="E39" s="31" t="s">
-        <v>189</v>
-      </c>
-      <c r="F39" s="43" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7">
-      <c r="A40" s="55"/>
-      <c r="B40" s="59"/>
-      <c r="C40" s="59"/>
-      <c r="D40" s="56"/>
-      <c r="E40" s="48" t="s">
-        <v>190</v>
-      </c>
-      <c r="F40" s="49" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7">
-      <c r="A41" s="55"/>
-      <c r="B41" s="59"/>
-      <c r="C41" s="59"/>
-      <c r="D41" s="32"/>
-      <c r="E41" s="31"/>
-      <c r="F41" s="41" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7">
-      <c r="A42" s="55"/>
-      <c r="B42" s="59"/>
-      <c r="C42" s="59"/>
-      <c r="D42" s="32"/>
-      <c r="E42" s="31"/>
-      <c r="F42" s="41" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7">
-      <c r="A43" s="55"/>
-      <c r="B43" s="59"/>
-      <c r="C43" s="59"/>
-      <c r="D43" s="50"/>
-      <c r="E43" s="50"/>
-      <c r="F43" s="41" t="s">
-        <v>198</v>
-      </c>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="55"/>
-      <c r="B44" s="59"/>
-      <c r="C44" s="54" t="s">
+      <c r="A44" s="58"/>
+      <c r="B44" s="56"/>
+      <c r="C44" s="53" t="s">
         <v>39</v>
       </c>
-      <c r="D44" s="32"/>
-      <c r="E44" s="32"/>
+      <c r="D44" s="31"/>
+      <c r="E44" s="31"/>
       <c r="F44" s="25" t="s">
         <v>40</v>
       </c>
       <c r="G44" s="11" t="s">
-        <v>199</v>
+        <v>185</v>
       </c>
     </row>
     <row r="45" spans="1:7">
-      <c r="A45" s="55"/>
-      <c r="B45" s="59"/>
-      <c r="C45" s="53"/>
-      <c r="D45" s="31" t="s">
-        <v>158</v>
-      </c>
-      <c r="E45" s="31"/>
+      <c r="A45" s="58"/>
+      <c r="B45" s="56"/>
+      <c r="C45" s="52"/>
+      <c r="D45" s="30" t="s">
+        <v>144</v>
+      </c>
+      <c r="E45" s="30"/>
       <c r="F45" s="26" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="46" spans="1:7">
-      <c r="A46" s="55"/>
-      <c r="B46" s="59"/>
-      <c r="C46" s="53"/>
-      <c r="D46" s="31" t="s">
+      <c r="A46" s="58"/>
+      <c r="B46" s="56"/>
+      <c r="C46" s="52"/>
+      <c r="D46" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="E46" s="31"/>
+      <c r="E46" s="30"/>
       <c r="F46" s="26" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
     </row>
     <row r="47" spans="1:7">
-      <c r="A47" s="55"/>
-      <c r="B47" s="59"/>
-      <c r="C47" s="53"/>
-      <c r="D47" s="31" t="s">
+      <c r="A47" s="58"/>
+      <c r="B47" s="56"/>
+      <c r="C47" s="52"/>
+      <c r="D47" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="E47" s="31"/>
+      <c r="E47" s="30"/>
       <c r="F47" s="26" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
     </row>
     <row r="48" spans="1:7">
-      <c r="A48" s="55"/>
-      <c r="B48" s="59"/>
-      <c r="C48" s="53"/>
-      <c r="D48" s="31" t="s">
-        <v>88</v>
-      </c>
-      <c r="E48" s="31"/>
+      <c r="A48" s="58"/>
+      <c r="B48" s="56"/>
+      <c r="C48" s="52"/>
+      <c r="D48" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="E48" s="30"/>
       <c r="F48" s="26" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A49" s="55"/>
-      <c r="B49" s="60"/>
-      <c r="C49" s="53"/>
-      <c r="D49" s="31" t="s">
-        <v>88</v>
-      </c>
-      <c r="E49" s="31"/>
+      <c r="A49" s="58"/>
+      <c r="B49" s="57"/>
+      <c r="C49" s="52"/>
+      <c r="D49" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="E49" s="30"/>
       <c r="F49" s="26" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="50" spans="1:7" s="36" customFormat="1" ht="15.75" thickTop="1">
-      <c r="A50" s="53" t="s">
+    <row r="50" spans="1:7" s="35" customFormat="1" ht="15.75" thickTop="1">
+      <c r="A50" s="52" t="s">
         <v>41</v>
       </c>
-      <c r="B50" s="33"/>
-      <c r="C50" s="33" t="s">
+      <c r="B50" s="32"/>
+      <c r="C50" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="D50" s="33"/>
-      <c r="E50" s="33"/>
-      <c r="F50" s="34" t="s">
+      <c r="D50" s="32"/>
+      <c r="E50" s="32"/>
+      <c r="F50" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="G50" s="35"/>
+      <c r="G50" s="34"/>
     </row>
     <row r="51" spans="1:7">
-      <c r="A51" s="53"/>
+      <c r="A51" s="52"/>
       <c r="B51" s="12"/>
       <c r="C51" s="5"/>
       <c r="D51" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="E51" s="40"/>
+      <c r="E51" s="39"/>
       <c r="F51" s="14" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="30">
-      <c r="A52" s="53"/>
+      <c r="A52" s="52"/>
       <c r="B52" s="12"/>
-      <c r="C52" s="53"/>
-      <c r="D52" s="53" t="s">
+      <c r="C52" s="52"/>
+      <c r="D52" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="E52" s="40"/>
+      <c r="E52" s="39"/>
       <c r="F52" s="14" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="53" spans="1:7">
-      <c r="A53" s="53"/>
+      <c r="A53" s="52"/>
       <c r="B53" s="12"/>
-      <c r="C53" s="53"/>
-      <c r="D53" s="53"/>
-      <c r="E53" s="40"/>
+      <c r="C53" s="52"/>
+      <c r="D53" s="52"/>
+      <c r="E53" s="39"/>
       <c r="F53" s="14" t="s">
-        <v>148</v>
+        <v>134</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="45">
-      <c r="A54" s="53"/>
+      <c r="A54" s="52"/>
       <c r="B54" s="12"/>
-      <c r="C54" s="53"/>
-      <c r="D54" s="53"/>
-      <c r="E54" s="40"/>
+      <c r="C54" s="52"/>
+      <c r="D54" s="52"/>
+      <c r="E54" s="39"/>
       <c r="F54" s="14" t="s">
-        <v>149</v>
+        <v>135</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A55" s="53"/>
+      <c r="A55" s="52"/>
       <c r="B55" s="12"/>
-      <c r="C55" s="53"/>
-      <c r="D55" s="53"/>
-      <c r="E55" s="40"/>
+      <c r="C55" s="52"/>
+      <c r="D55" s="52"/>
+      <c r="E55" s="39"/>
       <c r="F55" s="5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="56" spans="1:7" s="36" customFormat="1" ht="15.75" thickTop="1">
-      <c r="A56" s="53" t="s">
+    <row r="56" spans="1:7" s="35" customFormat="1" ht="15.75" thickTop="1">
+      <c r="A56" s="52" t="s">
         <v>47</v>
       </c>
-      <c r="B56" s="33"/>
-      <c r="C56" s="53"/>
-      <c r="D56" s="54" t="s">
+      <c r="B56" s="32"/>
+      <c r="C56" s="52"/>
+      <c r="D56" s="53" t="s">
         <v>19</v>
       </c>
-      <c r="E56" s="41"/>
-      <c r="F56" s="38" t="s">
-        <v>150</v>
-      </c>
-      <c r="G56" s="35"/>
+      <c r="E56" s="40"/>
+      <c r="F56" s="37" t="s">
+        <v>136</v>
+      </c>
+      <c r="G56" s="34"/>
     </row>
     <row r="57" spans="1:7">
-      <c r="A57" s="53"/>
+      <c r="A57" s="52"/>
       <c r="B57" s="12"/>
-      <c r="C57" s="53"/>
-      <c r="D57" s="53"/>
-      <c r="E57" s="40"/>
+      <c r="C57" s="52"/>
+      <c r="D57" s="52"/>
+      <c r="E57" s="39"/>
       <c r="F57" s="7" t="s">
-        <v>151</v>
+        <v>137</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="30">
-      <c r="A58" s="53"/>
+      <c r="A58" s="52"/>
       <c r="B58" s="12"/>
-      <c r="C58" s="53"/>
-      <c r="D58" s="53"/>
-      <c r="E58" s="40"/>
+      <c r="C58" s="52"/>
+      <c r="D58" s="52"/>
+      <c r="E58" s="39"/>
       <c r="F58" s="14" t="s">
-        <v>152</v>
+        <v>138</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="30">
-      <c r="A59" s="53"/>
+      <c r="A59" s="52"/>
       <c r="B59" s="12"/>
-      <c r="C59" s="53"/>
-      <c r="D59" s="53"/>
-      <c r="E59" s="40"/>
+      <c r="C59" s="52"/>
+      <c r="D59" s="52"/>
+      <c r="E59" s="39"/>
       <c r="F59" s="14" t="s">
-        <v>153</v>
+        <v>139</v>
       </c>
     </row>
     <row r="60" spans="1:7">
-      <c r="A60" s="53"/>
+      <c r="A60" s="52"/>
       <c r="B60" s="12"/>
-      <c r="C60" s="53"/>
-      <c r="D60" s="53"/>
-      <c r="E60" s="40"/>
+      <c r="C60" s="52"/>
+      <c r="D60" s="52"/>
+      <c r="E60" s="39"/>
       <c r="F60" s="5" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A61" s="53"/>
+      <c r="A61" s="52"/>
       <c r="B61" s="12"/>
       <c r="C61" s="5"/>
       <c r="D61" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E61" s="40"/>
+      <c r="E61" s="39"/>
       <c r="F61" s="25" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="62" spans="1:7" s="36" customFormat="1" ht="15.75" thickTop="1">
-      <c r="A62" s="53" t="s">
+    <row r="62" spans="1:7" s="35" customFormat="1" ht="15.75" thickTop="1">
+      <c r="A62" s="52" t="s">
         <v>50</v>
       </c>
-      <c r="B62" s="33"/>
-      <c r="C62" s="38" t="s">
+      <c r="B62" s="32"/>
+      <c r="C62" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="D62" s="38" t="s">
+      <c r="D62" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="E62" s="38"/>
-      <c r="F62" s="34" t="s">
+      <c r="E62" s="37"/>
+      <c r="F62" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="G62" s="35"/>
+      <c r="G62" s="34"/>
     </row>
     <row r="63" spans="1:7">
-      <c r="A63" s="53"/>
+      <c r="A63" s="52"/>
       <c r="B63" s="12"/>
-      <c r="C63" s="54" t="s">
-        <v>181</v>
+      <c r="C63" s="53" t="s">
+        <v>167</v>
       </c>
       <c r="D63" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="E63" s="46"/>
-      <c r="F63" s="39" t="s">
+      <c r="E63" s="45"/>
+      <c r="F63" s="38" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="64" spans="1:7">
-      <c r="A64" s="53"/>
+      <c r="A64" s="52"/>
       <c r="B64" s="12"/>
-      <c r="C64" s="53"/>
+      <c r="C64" s="52"/>
       <c r="D64" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="E64" s="46"/>
-      <c r="F64" s="39" t="s">
+      <c r="E64" s="45"/>
+      <c r="F64" s="38" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="65" spans="1:7">
-      <c r="A65" s="53"/>
+      <c r="A65" s="52"/>
       <c r="B65" s="12"/>
-      <c r="C65" s="53"/>
+      <c r="C65" s="52"/>
       <c r="D65" s="24" t="s">
-        <v>182</v>
-      </c>
-      <c r="E65" s="47"/>
-      <c r="F65" s="39" t="s">
+        <v>168</v>
+      </c>
+      <c r="E65" s="46"/>
+      <c r="F65" s="38" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="66" spans="1:7">
-      <c r="A66" s="53"/>
+      <c r="A66" s="52"/>
       <c r="B66" s="12"/>
-      <c r="C66" s="53"/>
+      <c r="C66" s="52"/>
       <c r="D66" s="12"/>
-      <c r="E66" s="46"/>
-      <c r="F66" s="39" t="s">
+      <c r="E66" s="45"/>
+      <c r="F66" s="38" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="67" spans="1:7">
-      <c r="A67" s="53"/>
+      <c r="A67" s="52"/>
       <c r="B67" s="12"/>
-      <c r="C67" s="57" t="s">
-        <v>180</v>
+      <c r="C67" s="54" t="s">
+        <v>166</v>
       </c>
       <c r="D67" s="27" t="s">
-        <v>179</v>
-      </c>
-      <c r="E67" s="43"/>
-      <c r="F67" s="44" t="s">
+        <v>165</v>
+      </c>
+      <c r="E67" s="42"/>
+      <c r="F67" s="43" t="s">
         <v>7</v>
       </c>
       <c r="G67" s="11" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
     </row>
     <row r="68" spans="1:7">
-      <c r="A68" s="53"/>
+      <c r="A68" s="52"/>
       <c r="B68" s="12"/>
-      <c r="C68" s="58"/>
+      <c r="C68" s="55"/>
       <c r="D68" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="E68" s="43"/>
-      <c r="F68" s="44">
+      <c r="E68" s="42"/>
+      <c r="F68" s="43">
         <v>2025</v>
       </c>
       <c r="G68" s="11" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="A62:A68"/>
-    <mergeCell ref="C63:C66"/>
-    <mergeCell ref="C67:C68"/>
-    <mergeCell ref="B18:B32"/>
-    <mergeCell ref="A50:A55"/>
-    <mergeCell ref="C52:C55"/>
-    <mergeCell ref="B33:B49"/>
-    <mergeCell ref="C33:C43"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A3:A7"/>
+    <mergeCell ref="C4:C7"/>
+    <mergeCell ref="D4:D7"/>
+    <mergeCell ref="A9:A17"/>
+    <mergeCell ref="C10:C15"/>
+    <mergeCell ref="D10:D15"/>
     <mergeCell ref="D52:D55"/>
     <mergeCell ref="A56:A61"/>
     <mergeCell ref="C56:C60"/>
@@ -2481,13 +2636,14 @@
     <mergeCell ref="D29:D32"/>
     <mergeCell ref="C44:C49"/>
     <mergeCell ref="D34:D40"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A3:A7"/>
-    <mergeCell ref="C4:C7"/>
-    <mergeCell ref="D4:D7"/>
-    <mergeCell ref="A9:A17"/>
-    <mergeCell ref="C10:C15"/>
-    <mergeCell ref="D10:D15"/>
+    <mergeCell ref="A62:A68"/>
+    <mergeCell ref="C63:C66"/>
+    <mergeCell ref="C67:C68"/>
+    <mergeCell ref="B18:B32"/>
+    <mergeCell ref="A50:A55"/>
+    <mergeCell ref="C52:C55"/>
+    <mergeCell ref="B33:B49"/>
+    <mergeCell ref="C33:C43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -2514,13 +2670,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="60" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
       <c r="F1" s="9"/>
     </row>
     <row r="2" spans="1:6" s="2" customFormat="1" ht="37.5" customHeight="1">
@@ -2555,59 +2711,59 @@
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="54"/>
+      <c r="A4" s="53"/>
       <c r="B4" s="14"/>
-      <c r="C4" s="54"/>
-      <c r="D4" s="54"/>
+      <c r="C4" s="53"/>
+      <c r="D4" s="53"/>
       <c r="E4" s="8" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="54"/>
+      <c r="A5" s="53"/>
       <c r="B5" s="14"/>
-      <c r="C5" s="54"/>
-      <c r="D5" s="54"/>
+      <c r="C5" s="53"/>
+      <c r="D5" s="53"/>
       <c r="E5" s="8" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="54"/>
+      <c r="A6" s="53"/>
       <c r="B6" s="14"/>
-      <c r="C6" s="54"/>
-      <c r="D6" s="54"/>
+      <c r="C6" s="53"/>
+      <c r="D6" s="53"/>
       <c r="E6" s="8" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="54"/>
+      <c r="A7" s="53"/>
       <c r="B7" s="14"/>
-      <c r="C7" s="54"/>
-      <c r="D7" s="54"/>
+      <c r="C7" s="53"/>
+      <c r="D7" s="53"/>
       <c r="E7" s="8" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="54" t="s">
+      <c r="A8" s="53" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="14"/>
-      <c r="C8" s="54" t="s">
-        <v>161</v>
-      </c>
-      <c r="D8" s="31"/>
+      <c r="C8" s="53" t="s">
+        <v>147</v>
+      </c>
+      <c r="D8" s="30"/>
       <c r="E8" s="8" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="54"/>
+      <c r="A9" s="53"/>
       <c r="B9" s="14"/>
-      <c r="C9" s="54"/>
-      <c r="D9" s="31" t="s">
+      <c r="C9" s="53"/>
+      <c r="D9" s="30" t="s">
         <v>18</v>
       </c>
       <c r="E9" s="14" t="s">
@@ -2615,87 +2771,87 @@
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="54"/>
+      <c r="A10" s="53"/>
       <c r="B10" s="14"/>
-      <c r="C10" s="54"/>
-      <c r="D10" s="31" t="s">
+      <c r="C10" s="53"/>
+      <c r="D10" s="30" t="s">
         <v>19</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="54"/>
+      <c r="A11" s="53"/>
       <c r="B11" s="14"/>
-      <c r="C11" s="54"/>
-      <c r="D11" s="31" t="s">
+      <c r="C11" s="53"/>
+      <c r="D11" s="30" t="s">
         <v>20</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>146</v>
+        <v>132</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="11" t="s">
-        <v>177</v>
+        <v>163</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>178</v>
-      </c>
-      <c r="C12" s="54" t="s">
+        <v>164</v>
+      </c>
+      <c r="C12" s="53" t="s">
         <v>67</v>
       </c>
-      <c r="D12" s="31" t="s">
+      <c r="D12" s="30" t="s">
         <v>19</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>174</v>
+        <v>160</v>
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="C13" s="54"/>
-      <c r="D13" s="31" t="s">
+      <c r="C13" s="53"/>
+      <c r="D13" s="30" t="s">
         <v>19</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="C14" s="54"/>
-      <c r="D14" s="31" t="s">
+      <c r="C14" s="53"/>
+      <c r="D14" s="30" t="s">
         <v>19</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>172</v>
+        <v>158</v>
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="C15" s="54"/>
-      <c r="D15" s="31" t="s">
+      <c r="C15" s="53"/>
+      <c r="D15" s="30" t="s">
         <v>19</v>
       </c>
       <c r="E15" s="14" t="s">
-        <v>171</v>
+        <v>157</v>
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="C16" s="54"/>
-      <c r="D16" s="31" t="s">
+      <c r="C16" s="53"/>
+      <c r="D16" s="30" t="s">
         <v>6</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>170</v>
+        <v>156</v>
       </c>
     </row>
     <row r="17" spans="1:5">
-      <c r="C17" s="54"/>
-      <c r="D17" s="31" t="s">
+      <c r="C17" s="53"/>
+      <c r="D17" s="30" t="s">
         <v>19</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -2703,105 +2859,105 @@
         <v>20</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
       <c r="D18" s="14"/>
       <c r="E18" s="14" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="54" t="s">
+      <c r="A19" s="53" t="s">
         <v>68</v>
       </c>
       <c r="B19" s="14"/>
-      <c r="C19" s="54"/>
-      <c r="D19" s="31" t="s">
+      <c r="C19" s="53"/>
+      <c r="D19" s="30" t="s">
         <v>43</v>
       </c>
       <c r="E19" s="14" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="54"/>
+      <c r="A20" s="53"/>
       <c r="B20" s="14"/>
-      <c r="C20" s="54"/>
-      <c r="D20" s="31" t="s">
+      <c r="C20" s="53"/>
+      <c r="D20" s="30" t="s">
         <v>6</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="54"/>
+      <c r="A21" s="53"/>
       <c r="B21" s="14"/>
-      <c r="C21" s="54"/>
-      <c r="D21" s="31" t="s">
+      <c r="C21" s="53"/>
+      <c r="D21" s="30" t="s">
         <v>19</v>
       </c>
       <c r="E21" s="14" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="54" t="s">
+      <c r="A22" s="53" t="s">
         <v>69</v>
       </c>
       <c r="B22" s="14"/>
-      <c r="C22" s="31"/>
-      <c r="D22" s="31" t="s">
-        <v>162</v>
+      <c r="C22" s="30"/>
+      <c r="D22" s="30" t="s">
+        <v>148</v>
       </c>
       <c r="E22" s="14" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="54"/>
+      <c r="A23" s="53"/>
       <c r="B23" s="14"/>
-      <c r="C23" s="31"/>
-      <c r="D23" s="31" t="s">
-        <v>162</v>
+      <c r="C23" s="30"/>
+      <c r="D23" s="30" t="s">
+        <v>148</v>
       </c>
       <c r="E23" s="14" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:5">
-      <c r="A24" s="54"/>
+      <c r="A24" s="53"/>
       <c r="B24" s="14"/>
-      <c r="C24" s="31"/>
-      <c r="D24" s="31" t="s">
+      <c r="C24" s="30"/>
+      <c r="D24" s="30" t="s">
         <v>20</v>
       </c>
       <c r="E24" s="14" t="s">
-        <v>165</v>
+        <v>151</v>
       </c>
     </row>
     <row r="25" spans="1:5">
-      <c r="A25" s="54"/>
+      <c r="A25" s="53"/>
       <c r="B25" s="14"/>
-      <c r="C25" s="31" t="s">
+      <c r="C25" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="D25" s="31" t="s">
+      <c r="D25" s="30" t="s">
         <v>6</v>
       </c>
       <c r="E25" s="14" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
     </row>
     <row r="26" spans="1:5">
-      <c r="A26" s="54"/>
+      <c r="A26" s="53"/>
       <c r="B26" s="14"/>
-      <c r="C26" s="31"/>
-      <c r="D26" s="31" t="s">
+      <c r="C26" s="30"/>
+      <c r="D26" s="30" t="s">
         <v>6</v>
       </c>
       <c r="E26" s="14" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -2818,25 +2974,25 @@
       </c>
     </row>
     <row r="28" spans="1:5">
-      <c r="A28" s="54"/>
-      <c r="B28" s="54"/>
-      <c r="C28" s="54"/>
-      <c r="D28" s="54"/>
-      <c r="E28" s="54"/>
+      <c r="A28" s="53"/>
+      <c r="B28" s="53"/>
+      <c r="C28" s="53"/>
+      <c r="D28" s="53"/>
+      <c r="E28" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A22:A26"/>
-    <mergeCell ref="A28:E28"/>
-    <mergeCell ref="C12:C17"/>
-    <mergeCell ref="A19:A21"/>
-    <mergeCell ref="C19:C21"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A4:A7"/>
     <mergeCell ref="C4:C7"/>
     <mergeCell ref="D4:D7"/>
     <mergeCell ref="A8:A11"/>
     <mergeCell ref="C8:C11"/>
+    <mergeCell ref="A22:A26"/>
+    <mergeCell ref="A28:E28"/>
+    <mergeCell ref="C12:C17"/>
+    <mergeCell ref="A19:A21"/>
+    <mergeCell ref="C19:C21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -2864,475 +3020,475 @@
   <sheetData>
     <row r="2" spans="1:6">
       <c r="A2" s="17" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="17" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="17" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="C4" s="18"/>
       <c r="D4" s="18"/>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="17" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="D5" s="20"/>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="17" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
       <c r="D6" s="20"/>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="17" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="D7" s="20"/>
       <c r="F7" s="22" t="s">
-        <v>138</v>
+        <v>124</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="17" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="C9" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="B9" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="C9" s="17" t="s">
-        <v>105</v>
-      </c>
       <c r="D9" s="19" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="B10" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="B10" s="17" t="s">
-        <v>105</v>
-      </c>
       <c r="C10" s="20" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="D10" s="20"/>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="C11" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="C11" s="17" t="s">
-        <v>105</v>
-      </c>
       <c r="D11" s="19" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
       <c r="F11" s="23" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="17" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="17" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="B13" s="18" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="C13" s="18"/>
       <c r="D13" s="18"/>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="17" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="C14" s="20" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="D14" s="20"/>
       <c r="F14" s="23" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="17" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="C16" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="B16" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="C16" s="17" t="s">
-        <v>105</v>
-      </c>
       <c r="D16" s="19" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="17" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="C17" s="20" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
       <c r="D17" s="20"/>
       <c r="F17" s="23" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="17" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="17" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="D19" s="19" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="17" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="D20" s="19" t="s">
-        <v>129</v>
+        <v>115</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="B21" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="C21" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="B21" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="C21" s="17" t="s">
-        <v>105</v>
-      </c>
       <c r="D21" s="19" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="17" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="B22" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="C22" s="20" t="s">
         <v>104</v>
-      </c>
-      <c r="C22" s="20" t="s">
-        <v>118</v>
       </c>
       <c r="D22" s="20"/>
       <c r="F22" s="23" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="17" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="D23" s="21" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="B24" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="C24" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="B24" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="C24" s="17" t="s">
-        <v>105</v>
-      </c>
       <c r="D24" s="19" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="17" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="B25" s="17" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="C25" s="20" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="D25" s="20"/>
       <c r="F25" s="23" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="B26" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="C26" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="B26" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="C26" s="17" t="s">
-        <v>105</v>
-      </c>
       <c r="D26" s="19" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="17" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="B27" s="17" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="C27" s="20" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="D27" s="20"/>
       <c r="F27" s="23" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="17" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="B28" s="17" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="D28" s="19" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="17" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="B29" s="17" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="C29" s="17" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="D29" s="19" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
       <c r="F29" s="23" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="17" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="B30" s="17" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="C30" s="17" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="D30" s="19" t="s">
-        <v>136</v>
+        <v>122</v>
       </c>
       <c r="F30" s="23" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="B31" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="C31" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="B31" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="C31" s="17" t="s">
-        <v>105</v>
-      </c>
       <c r="D31" s="19" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="F31" s="23" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="17" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="B32" s="17" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="C32" s="20" t="s">
-        <v>121</v>
+        <v>107</v>
       </c>
       <c r="D32" s="20"/>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="17" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="B33" s="17" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="C33" s="20" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="D33" s="20"/>
       <c r="F33" s="23" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="B34" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="B34" s="17" t="s">
-        <v>105</v>
-      </c>
       <c r="C34" s="20" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="D34" s="20"/>
       <c r="F34" s="23" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="17" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" s="17" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="B36" s="18" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" s="17" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="B37" s="18" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
     </row>
     <row r="38" spans="1:6">
       <c r="A38" s="17" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="B38" s="18" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
     </row>
     <row r="39" spans="1:6">
       <c r="A39" s="17" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="B39" s="18" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -3343,323 +3499,559 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="27" customWidth="1"/>
-    <col min="2" max="2" width="44" customWidth="1"/>
-    <col min="3" max="3" width="37.85546875" customWidth="1"/>
-    <col min="4" max="4" width="87.5703125" customWidth="1"/>
-    <col min="5" max="5" width="43.5703125" customWidth="1"/>
+    <col min="1" max="1" width="4.7109375" style="63" customWidth="1"/>
+    <col min="2" max="2" width="41.85546875" style="63" customWidth="1"/>
+    <col min="3" max="3" width="37.85546875" style="63" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" style="63" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="52.5703125" style="63" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="63"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" ht="37.5" customHeight="1">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:5" s="66" customFormat="1" ht="37.5" customHeight="1">
+      <c r="A1" s="51" t="s">
+        <v>213</v>
+      </c>
+      <c r="B1" s="51" t="s">
+        <v>228</v>
+      </c>
+      <c r="C1" s="51" t="s">
+        <v>227</v>
+      </c>
+      <c r="D1" s="64" t="s">
+        <v>211</v>
+      </c>
+      <c r="E1" s="65" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="51">
+        <v>0</v>
+      </c>
+      <c r="B2" s="51" t="s">
+        <v>215</v>
+      </c>
+      <c r="C2" s="67" t="s">
+        <v>210</v>
+      </c>
+      <c r="D2" s="63" t="s">
+        <v>225</v>
+      </c>
+      <c r="E2" s="63" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="51">
+        <f>SUM(A2+1)</f>
         <v>1</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B3" s="51" t="s">
+        <v>216</v>
+      </c>
+      <c r="C3" s="67" t="s">
+        <v>210</v>
+      </c>
+      <c r="D3" s="63" t="s">
+        <v>225</v>
+      </c>
+      <c r="E3" s="63" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="51">
+        <f>SUM(A3+1)</f>
         <v>2</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="B4" s="51" t="s">
+        <v>217</v>
+      </c>
+      <c r="C4" s="67" t="s">
+        <v>210</v>
+      </c>
+      <c r="D4" s="63" t="s">
+        <v>225</v>
+      </c>
+      <c r="E4" s="63" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="51">
+        <f t="shared" ref="A5:A30" si="0">SUM(A4+1)</f>
         <v>3</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="B5" s="51" t="s">
+        <v>224</v>
+      </c>
+      <c r="C5" s="67" t="s">
+        <v>210</v>
+      </c>
+      <c r="D5" s="63" t="s">
+        <v>225</v>
+      </c>
+      <c r="E5" s="63" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="51">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="B6" s="51" t="s">
+        <v>218</v>
+      </c>
+      <c r="C6" s="67" t="s">
+        <v>210</v>
+      </c>
+      <c r="D6" s="63" t="s">
+        <v>225</v>
+      </c>
+      <c r="E6" s="63" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="51">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B7" s="51" t="s">
+        <v>219</v>
+      </c>
+      <c r="C7" s="67" t="s">
+        <v>210</v>
+      </c>
+      <c r="D7" s="63" t="s">
+        <v>225</v>
+      </c>
+      <c r="E7" s="63" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="51">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B8" s="51" t="s">
+        <v>214</v>
+      </c>
+      <c r="C8" s="67" t="s">
+        <v>210</v>
+      </c>
+      <c r="D8" s="63" t="s">
+        <v>225</v>
+      </c>
+      <c r="E8" s="63" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="51">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B9" s="51" t="s">
+        <v>220</v>
+      </c>
+      <c r="C9" s="67" t="s">
+        <v>210</v>
+      </c>
+      <c r="D9" s="63" t="s">
+        <v>225</v>
+      </c>
+      <c r="E9" s="63" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="51">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B10" s="51" t="s">
+        <v>221</v>
+      </c>
+      <c r="C10" s="67" t="s">
+        <v>210</v>
+      </c>
+      <c r="D10" s="63" t="s">
+        <v>225</v>
+      </c>
+      <c r="E10" s="63" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="51">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B11" s="51" t="s">
+        <v>222</v>
+      </c>
+      <c r="C11" s="67" t="s">
+        <v>210</v>
+      </c>
+      <c r="D11" s="63" t="s">
+        <v>225</v>
+      </c>
+      <c r="E11" s="63" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="51">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B12" s="51" t="s">
+        <v>223</v>
+      </c>
+      <c r="C12" s="67" t="s">
+        <v>210</v>
+      </c>
+      <c r="D12" s="63" t="s">
+        <v>225</v>
+      </c>
+      <c r="E12" s="63" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="51">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B13" s="51" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="67" t="s">
+        <v>200</v>
+      </c>
+      <c r="D13" s="63" t="s">
+        <v>226</v>
+      </c>
+      <c r="E13" s="63" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="51">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B14" s="51" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="67" t="s">
+        <v>200</v>
+      </c>
+      <c r="D14" s="63" t="s">
+        <v>226</v>
+      </c>
+      <c r="E14" s="63" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="51">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B15" s="51" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="67" t="s">
+        <v>200</v>
+      </c>
+      <c r="D15" s="63" t="s">
+        <v>226</v>
+      </c>
+      <c r="E15" s="63" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="51">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B16" s="51" t="s">
+        <v>71</v>
+      </c>
+      <c r="C16" s="67" t="s">
+        <v>200</v>
+      </c>
+      <c r="D16" s="63" t="s">
+        <v>226</v>
+      </c>
+      <c r="E16" s="63" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="51">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B17" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="67" t="s">
+        <v>200</v>
+      </c>
+      <c r="D17" s="63" t="s">
+        <v>226</v>
+      </c>
+      <c r="E17" s="63" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="51">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B18" s="51" t="s">
+        <v>72</v>
+      </c>
+      <c r="C18" s="67" t="s">
+        <v>200</v>
+      </c>
+      <c r="D18" s="63" t="s">
+        <v>226</v>
+      </c>
+      <c r="E18" s="63" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="51">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B19" s="51" t="s">
+        <v>73</v>
+      </c>
+      <c r="C19" s="67" t="s">
+        <v>200</v>
+      </c>
+      <c r="D19" s="63" t="s">
+        <v>226</v>
+      </c>
+      <c r="E19" s="63" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="51">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B20" s="51" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="67" t="s">
+        <v>200</v>
+      </c>
+      <c r="D20" s="63" t="s">
+        <v>226</v>
+      </c>
+      <c r="E20" s="63" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="51">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B21" s="51" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" s="67" t="s">
+        <v>201</v>
+      </c>
+      <c r="D21" s="63" t="s">
+        <v>226</v>
+      </c>
+      <c r="E21" s="63" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="51">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B22" s="51" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" s="67" t="s">
+        <v>201</v>
+      </c>
+      <c r="D22" s="63" t="s">
+        <v>226</v>
+      </c>
+      <c r="E22" s="63" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="51">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="B23" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" s="67" t="s">
+        <v>201</v>
+      </c>
+      <c r="D23" s="63" t="s">
+        <v>226</v>
+      </c>
+      <c r="E23" s="63" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="51">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B24" s="51" t="s">
+        <v>37</v>
+      </c>
+      <c r="C24" s="67" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="54"/>
-      <c r="B2" s="54" t="s">
-        <v>70</v>
-      </c>
-      <c r="C2" s="54"/>
-      <c r="D2" s="8" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" s="63" customFormat="1">
-      <c r="A3" s="54"/>
-      <c r="B3" s="54"/>
-      <c r="C3" s="54"/>
-      <c r="D3" s="62" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="54"/>
-      <c r="B4" s="54"/>
-      <c r="C4" s="54"/>
-      <c r="D4" s="8" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" s="63" customFormat="1">
-      <c r="A5" s="54"/>
-      <c r="B5" s="54"/>
-      <c r="C5" s="54"/>
-      <c r="D5" s="62" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="54"/>
-      <c r="B6" s="54"/>
-      <c r="C6" s="54"/>
-      <c r="D6" s="8" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" s="63" customFormat="1">
-      <c r="A7" s="54"/>
-      <c r="B7" s="54"/>
-      <c r="C7" s="54"/>
-      <c r="D7" s="62" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="54"/>
-      <c r="B8" s="54"/>
-      <c r="C8" s="54"/>
-      <c r="D8" s="8" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" s="63" customFormat="1">
-      <c r="A9" s="54"/>
-      <c r="B9" s="54"/>
-      <c r="C9" s="54"/>
-      <c r="D9" s="62" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="54"/>
-      <c r="B10" s="54"/>
-      <c r="C10" s="54"/>
-      <c r="D10" s="8" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" s="63" customFormat="1">
-      <c r="A11" s="54"/>
-      <c r="B11" s="54"/>
-      <c r="C11" s="54"/>
-      <c r="D11" s="62" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="54"/>
-      <c r="B12" s="54"/>
-      <c r="C12" s="54"/>
-      <c r="D12" s="8" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="61"/>
-      <c r="B13" s="61"/>
-      <c r="C13" s="61"/>
-      <c r="D13" s="61"/>
-    </row>
-    <row r="14" spans="1:5" s="63" customFormat="1">
-      <c r="A14" s="54"/>
-      <c r="B14" s="54" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" s="54" t="s">
-        <v>82</v>
-      </c>
-      <c r="D14" s="62" t="s">
+      <c r="D24" s="63" t="s">
+        <v>226</v>
+      </c>
+      <c r="E24" s="63" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="51">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="B25" s="51" t="s">
+        <v>35</v>
+      </c>
+      <c r="C25" s="67" t="s">
+        <v>202</v>
+      </c>
+      <c r="D25" s="63" t="s">
+        <v>226</v>
+      </c>
+      <c r="E25" s="63" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="51">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="B26" s="51" t="s">
+        <v>38</v>
+      </c>
+      <c r="C26" s="67" t="s">
+        <v>202</v>
+      </c>
+      <c r="D26" s="63" t="s">
+        <v>226</v>
+      </c>
+      <c r="E26" s="63" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="51">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="B27" s="51" t="s">
+        <v>36</v>
+      </c>
+      <c r="C27" s="67" t="s">
+        <v>202</v>
+      </c>
+      <c r="D27" s="63" t="s">
+        <v>226</v>
+      </c>
+      <c r="E27" s="63" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="51">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="B28" s="63" t="s">
+        <v>207</v>
+      </c>
+      <c r="C28" s="63" t="s">
+        <v>209</v>
+      </c>
+      <c r="D28" s="63" t="s">
+        <v>225</v>
+      </c>
+      <c r="E28" s="63" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="51">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="B29" s="63" t="s">
+        <v>208</v>
+      </c>
+      <c r="C29" s="63" t="s">
+        <v>209</v>
+      </c>
+      <c r="D29" s="63" t="s">
+        <v>225</v>
+      </c>
+      <c r="E29" s="63" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="51">
+        <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="E14" s="63" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="54"/>
-      <c r="B15" s="54"/>
-      <c r="C15" s="54"/>
-      <c r="D15" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E15" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" s="63" customFormat="1">
-      <c r="A16" s="54"/>
-      <c r="B16" s="54"/>
-      <c r="C16" s="54"/>
-      <c r="D16" s="62" t="s">
-        <v>26</v>
-      </c>
-      <c r="E16" s="63" t="s">
+      <c r="B30" s="63" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="54"/>
-      <c r="B17" s="54"/>
-      <c r="C17" s="54"/>
-      <c r="D17" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="E17" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" s="63" customFormat="1">
-      <c r="A18" s="54"/>
-      <c r="B18" s="54"/>
-      <c r="C18" s="54"/>
-      <c r="D18" s="62" t="s">
-        <v>24</v>
-      </c>
-      <c r="E18" s="63" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="54"/>
-      <c r="B19" s="54"/>
-      <c r="C19" s="54"/>
-      <c r="D19" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="E19" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" s="63" customFormat="1">
-      <c r="A20" s="54"/>
-      <c r="B20" s="54"/>
-      <c r="C20" s="54"/>
-      <c r="D20" s="62" t="s">
-        <v>85</v>
-      </c>
-      <c r="E20" s="63" t="s">
+      <c r="C30" s="63" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="54"/>
-      <c r="B21" s="54"/>
-      <c r="C21" s="54"/>
-      <c r="D21" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E21" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" s="63" customFormat="1">
-      <c r="A22" s="54"/>
-      <c r="B22" s="54"/>
-      <c r="C22" s="54" t="s">
-        <v>86</v>
-      </c>
-      <c r="D22" s="62" t="s">
-        <v>31</v>
-      </c>
-      <c r="E22" s="63" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23" s="54"/>
-      <c r="B23" s="54"/>
-      <c r="C23" s="54"/>
-      <c r="D23" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="E23" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" s="63" customFormat="1">
-      <c r="A24" s="54"/>
-      <c r="B24" s="54"/>
-      <c r="C24" s="54"/>
-      <c r="D24" s="62" t="s">
-        <v>33</v>
-      </c>
-      <c r="E24" s="63" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25" s="54"/>
-      <c r="B25" s="54"/>
-      <c r="C25" s="54" t="s">
-        <v>87</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="E25" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" s="63" customFormat="1">
-      <c r="A26" s="54"/>
-      <c r="B26" s="54"/>
-      <c r="C26" s="54"/>
-      <c r="D26" s="62" t="s">
-        <v>35</v>
-      </c>
-      <c r="E26" s="63" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27" s="54"/>
-      <c r="B27" s="54"/>
-      <c r="C27" s="54"/>
-      <c r="D27" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="E27" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" s="63" customFormat="1">
-      <c r="A28" s="54"/>
-      <c r="B28" s="54"/>
-      <c r="C28" s="54"/>
-      <c r="D28" s="62" t="s">
-        <v>36</v>
-      </c>
-      <c r="E28" s="63" t="s">
-        <v>212</v>
+      <c r="D30" s="63" t="s">
+        <v>225</v>
+      </c>
+      <c r="E30" s="63" t="s">
+        <v>242</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="A2:A12"/>
-    <mergeCell ref="B2:B12"/>
-    <mergeCell ref="C2:C12"/>
-    <mergeCell ref="A25:A28"/>
-    <mergeCell ref="B25:B28"/>
-    <mergeCell ref="C25:C28"/>
-    <mergeCell ref="A13:D13"/>
-    <mergeCell ref="A14:A21"/>
-    <mergeCell ref="B14:B21"/>
-    <mergeCell ref="C14:C21"/>
-    <mergeCell ref="A22:A24"/>
-    <mergeCell ref="B22:B24"/>
-    <mergeCell ref="C22:C24"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
@@ -3667,9 +4059,198 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E22"/>
+  <sheetViews>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="69"/>
+    <col min="2" max="2" width="41.85546875" style="69" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12" style="69" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" style="69" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="69" t="s">
+        <v>213</v>
+      </c>
+      <c r="B1" s="69" t="s">
+        <v>250</v>
+      </c>
+      <c r="C1" s="69" t="s">
+        <v>251</v>
+      </c>
+      <c r="D1" s="69" t="s">
+        <v>196</v>
+      </c>
+      <c r="E1" s="69" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="69">
+        <v>0</v>
+      </c>
+      <c r="B2" s="69" t="s">
+        <v>180</v>
+      </c>
+      <c r="C2" s="69">
+        <v>1945</v>
+      </c>
+      <c r="D2" s="69" t="s">
+        <v>179</v>
+      </c>
+      <c r="E2" s="69" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="69">
+        <f>SUM(A2+1)</f>
+        <v>1</v>
+      </c>
+      <c r="B3" s="69" t="s">
+        <v>253</v>
+      </c>
+      <c r="C3" s="69" t="s">
+        <v>247</v>
+      </c>
+      <c r="D3" s="69" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="69" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="69">
+        <f t="shared" ref="A4:A5" si="0">SUM(A3+1)</f>
+        <v>2</v>
+      </c>
+      <c r="B4" s="69" t="s">
+        <v>244</v>
+      </c>
+      <c r="C4" s="69" t="s">
+        <v>248</v>
+      </c>
+      <c r="D4" s="69" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="69">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="69">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="B5" s="69" t="s">
+        <v>246</v>
+      </c>
+      <c r="C5" s="69" t="s">
+        <v>249</v>
+      </c>
+      <c r="D5" s="69" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="69" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="70"/>
+      <c r="D14" s="71"/>
+      <c r="E14" s="70"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="70"/>
+      <c r="D15" s="71"/>
+      <c r="E15" s="70"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="70"/>
+      <c r="D16" s="70"/>
+      <c r="E16" s="70"/>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="70"/>
+      <c r="D17" s="71"/>
+      <c r="E17" s="70"/>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="70"/>
+      <c r="D18" s="72"/>
+      <c r="E18" s="70"/>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="70"/>
+      <c r="D19" s="71"/>
+      <c r="E19" s="70"/>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="70"/>
+      <c r="D20" s="71"/>
+      <c r="E20" s="70"/>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="70"/>
+      <c r="D21" s="71"/>
+      <c r="E21" s="70"/>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="70"/>
+      <c r="D22" s="71"/>
+      <c r="E22" s="70"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A2:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>203</v>
+      </c>
+      <c r="B2" s="62" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="B3" s="62" t="s">
+        <v>205</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C23" sqref="C23:C28"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>

</xml_diff>

<commit_message>
.json files for mainPage copy
</commit_message>
<xml_diff>
--- a/03_design/architecture-copy.xlsx
+++ b/03_design/architecture-copy.xlsx
@@ -1440,36 +1440,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1498,6 +1468,36 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1796,8 +1796,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33:B49"/>
+    <sheetView tabSelected="1" topLeftCell="B46" workbookViewId="0">
+      <selection activeCell="F63" sqref="F63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1812,14 +1812,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
       <c r="G1" s="3"/>
     </row>
     <row r="2" spans="1:7" ht="37.5" customHeight="1" thickBot="1">
@@ -1842,7 +1842,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" s="35" customFormat="1" ht="15.75" thickTop="1">
-      <c r="A3" s="52" t="s">
+      <c r="A3" s="65" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="32"/>
@@ -1856,12 +1856,12 @@
       <c r="G3" s="34"/>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="52"/>
+      <c r="A4" s="65"/>
       <c r="B4" s="12"/>
-      <c r="C4" s="52" t="s">
+      <c r="C4" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="52" t="s">
+      <c r="D4" s="65" t="s">
         <v>9</v>
       </c>
       <c r="E4" s="39"/>
@@ -1870,30 +1870,30 @@
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="52"/>
+      <c r="A5" s="65"/>
       <c r="B5" s="12"/>
-      <c r="C5" s="52"/>
-      <c r="D5" s="52"/>
+      <c r="C5" s="65"/>
+      <c r="D5" s="65"/>
       <c r="E5" s="39"/>
       <c r="F5" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="52"/>
+      <c r="A6" s="65"/>
       <c r="B6" s="12"/>
-      <c r="C6" s="52"/>
-      <c r="D6" s="52"/>
+      <c r="C6" s="65"/>
+      <c r="D6" s="65"/>
       <c r="E6" s="39"/>
       <c r="F6" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="52"/>
+      <c r="A7" s="65"/>
       <c r="B7" s="12"/>
-      <c r="C7" s="52"/>
-      <c r="D7" s="52"/>
+      <c r="C7" s="65"/>
+      <c r="D7" s="65"/>
       <c r="E7" s="39"/>
       <c r="F7" s="5" t="s">
         <v>13</v>
@@ -1910,7 +1910,7 @@
       <c r="F8" s="44"/>
     </row>
     <row r="9" spans="1:7" s="35" customFormat="1" ht="15.75" thickTop="1">
-      <c r="A9" s="52" t="s">
+      <c r="A9" s="65" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="32"/>
@@ -1925,12 +1925,12 @@
       <c r="G9" s="34"/>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="52"/>
+      <c r="A10" s="65"/>
       <c r="B10" s="12"/>
-      <c r="C10" s="52" t="s">
+      <c r="C10" s="65" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="52" t="s">
+      <c r="D10" s="65" t="s">
         <v>18</v>
       </c>
       <c r="E10" s="39"/>
@@ -1939,57 +1939,57 @@
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="52"/>
+      <c r="A11" s="65"/>
       <c r="B11" s="12"/>
-      <c r="C11" s="52"/>
-      <c r="D11" s="52"/>
+      <c r="C11" s="65"/>
+      <c r="D11" s="65"/>
       <c r="E11" s="39"/>
       <c r="F11" s="26" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="52"/>
+      <c r="A12" s="65"/>
       <c r="B12" s="12"/>
-      <c r="C12" s="52"/>
-      <c r="D12" s="52"/>
+      <c r="C12" s="65"/>
+      <c r="D12" s="65"/>
       <c r="E12" s="39"/>
       <c r="F12" s="26" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="52"/>
+      <c r="A13" s="65"/>
       <c r="B13" s="12"/>
-      <c r="C13" s="52"/>
-      <c r="D13" s="52"/>
+      <c r="C13" s="65"/>
+      <c r="D13" s="65"/>
       <c r="E13" s="39"/>
       <c r="F13" s="26" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="52"/>
+      <c r="A14" s="65"/>
       <c r="B14" s="12"/>
-      <c r="C14" s="52"/>
-      <c r="D14" s="52"/>
+      <c r="C14" s="65"/>
+      <c r="D14" s="65"/>
       <c r="E14" s="39"/>
       <c r="F14" s="26" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="52"/>
+      <c r="A15" s="65"/>
       <c r="B15" s="12"/>
-      <c r="C15" s="52"/>
-      <c r="D15" s="52"/>
+      <c r="C15" s="65"/>
+      <c r="D15" s="65"/>
       <c r="E15" s="39"/>
       <c r="F15" s="26" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="52"/>
+      <c r="A16" s="65"/>
       <c r="B16" s="12"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5" t="s">
@@ -2001,7 +2001,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A17" s="52"/>
+      <c r="A17" s="65"/>
       <c r="B17" s="12"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5" t="s">
@@ -2013,16 +2013,16 @@
       </c>
     </row>
     <row r="18" spans="1:7" s="35" customFormat="1" ht="15.75" thickTop="1">
-      <c r="A18" s="58" t="s">
+      <c r="A18" s="67" t="s">
         <v>143</v>
       </c>
-      <c r="B18" s="53" t="s">
+      <c r="B18" s="66" t="s">
         <v>142</v>
       </c>
-      <c r="C18" s="52" t="s">
+      <c r="C18" s="65" t="s">
         <v>22</v>
       </c>
-      <c r="D18" s="53" t="s">
+      <c r="D18" s="66" t="s">
         <v>23</v>
       </c>
       <c r="E18" s="40"/>
@@ -2032,80 +2032,80 @@
       <c r="G18" s="34"/>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="58"/>
-      <c r="B19" s="53"/>
-      <c r="C19" s="52"/>
-      <c r="D19" s="53"/>
+      <c r="A19" s="67"/>
+      <c r="B19" s="66"/>
+      <c r="C19" s="65"/>
+      <c r="D19" s="66"/>
       <c r="E19" s="40"/>
       <c r="F19" s="14" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="58"/>
-      <c r="B20" s="53"/>
-      <c r="C20" s="52"/>
-      <c r="D20" s="52"/>
+      <c r="A20" s="67"/>
+      <c r="B20" s="66"/>
+      <c r="C20" s="65"/>
+      <c r="D20" s="65"/>
       <c r="E20" s="39"/>
       <c r="F20" s="14" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="58"/>
-      <c r="B21" s="53"/>
-      <c r="C21" s="52"/>
-      <c r="D21" s="52"/>
+      <c r="A21" s="67"/>
+      <c r="B21" s="66"/>
+      <c r="C21" s="65"/>
+      <c r="D21" s="65"/>
       <c r="E21" s="39"/>
       <c r="F21" s="14" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="58"/>
-      <c r="B22" s="53"/>
-      <c r="C22" s="52"/>
-      <c r="D22" s="52"/>
+      <c r="A22" s="67"/>
+      <c r="B22" s="66"/>
+      <c r="C22" s="65"/>
+      <c r="D22" s="65"/>
       <c r="E22" s="39"/>
       <c r="F22" s="14" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" s="58"/>
-      <c r="B23" s="53"/>
-      <c r="C23" s="52"/>
-      <c r="D23" s="52"/>
+      <c r="A23" s="67"/>
+      <c r="B23" s="66"/>
+      <c r="C23" s="65"/>
+      <c r="D23" s="65"/>
       <c r="E23" s="39"/>
       <c r="F23" s="14" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:7">
-      <c r="A24" s="58"/>
-      <c r="B24" s="53"/>
-      <c r="C24" s="52"/>
-      <c r="D24" s="52"/>
+      <c r="A24" s="67"/>
+      <c r="B24" s="66"/>
+      <c r="C24" s="65"/>
+      <c r="D24" s="65"/>
       <c r="E24" s="39"/>
       <c r="F24" s="26" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="25" spans="1:7">
-      <c r="A25" s="58"/>
-      <c r="B25" s="53"/>
-      <c r="C25" s="52"/>
-      <c r="D25" s="52"/>
+      <c r="A25" s="67"/>
+      <c r="B25" s="66"/>
+      <c r="C25" s="65"/>
+      <c r="D25" s="65"/>
       <c r="E25" s="39"/>
       <c r="F25" s="14" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="58"/>
-      <c r="B26" s="53"/>
-      <c r="C26" s="52"/>
-      <c r="D26" s="53" t="s">
+      <c r="A26" s="67"/>
+      <c r="B26" s="66"/>
+      <c r="C26" s="65"/>
+      <c r="D26" s="66" t="s">
         <v>30</v>
       </c>
       <c r="E26" s="40"/>
@@ -2114,30 +2114,30 @@
       </c>
     </row>
     <row r="27" spans="1:7">
-      <c r="A27" s="58"/>
-      <c r="B27" s="53"/>
-      <c r="C27" s="52"/>
-      <c r="D27" s="52"/>
+      <c r="A27" s="67"/>
+      <c r="B27" s="66"/>
+      <c r="C27" s="65"/>
+      <c r="D27" s="65"/>
       <c r="E27" s="39"/>
       <c r="F27" s="14" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" s="58"/>
-      <c r="B28" s="53"/>
-      <c r="C28" s="52"/>
-      <c r="D28" s="52"/>
+      <c r="A28" s="67"/>
+      <c r="B28" s="66"/>
+      <c r="C28" s="65"/>
+      <c r="D28" s="65"/>
       <c r="E28" s="39"/>
       <c r="F28" s="14" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="29" spans="1:7">
-      <c r="A29" s="58"/>
-      <c r="B29" s="53"/>
-      <c r="C29" s="52"/>
-      <c r="D29" s="53" t="s">
+      <c r="A29" s="67"/>
+      <c r="B29" s="66"/>
+      <c r="C29" s="65"/>
+      <c r="D29" s="66" t="s">
         <v>34</v>
       </c>
       <c r="E29" s="40"/>
@@ -2146,41 +2146,41 @@
       </c>
     </row>
     <row r="30" spans="1:7">
-      <c r="A30" s="58"/>
-      <c r="B30" s="53"/>
-      <c r="C30" s="52"/>
-      <c r="D30" s="52"/>
+      <c r="A30" s="67"/>
+      <c r="B30" s="66"/>
+      <c r="C30" s="65"/>
+      <c r="D30" s="65"/>
       <c r="E30" s="39"/>
       <c r="F30" s="14" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="31" spans="1:7">
-      <c r="A31" s="58"/>
-      <c r="B31" s="53"/>
-      <c r="C31" s="52"/>
-      <c r="D31" s="52"/>
+      <c r="A31" s="67"/>
+      <c r="B31" s="66"/>
+      <c r="C31" s="65"/>
+      <c r="D31" s="65"/>
       <c r="E31" s="39"/>
       <c r="F31" s="14" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="32" spans="1:7">
-      <c r="A32" s="58"/>
-      <c r="B32" s="53"/>
-      <c r="C32" s="52"/>
-      <c r="D32" s="52"/>
+      <c r="A32" s="67"/>
+      <c r="B32" s="66"/>
+      <c r="C32" s="65"/>
+      <c r="D32" s="65"/>
       <c r="E32" s="39"/>
       <c r="F32" s="14" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="33" spans="1:7">
-      <c r="A33" s="58"/>
-      <c r="B33" s="56" t="s">
+      <c r="A33" s="67"/>
+      <c r="B33" s="71" t="s">
         <v>21</v>
       </c>
-      <c r="C33" s="56" t="s">
+      <c r="C33" s="71" t="s">
         <v>169</v>
       </c>
       <c r="D33" s="40" t="s">
@@ -2190,25 +2190,25 @@
       <c r="F33" s="40"/>
     </row>
     <row r="34" spans="1:7" s="29" customFormat="1">
-      <c r="A34" s="58"/>
-      <c r="B34" s="56"/>
-      <c r="C34" s="56"/>
-      <c r="D34" s="53" t="s">
+      <c r="A34" s="67"/>
+      <c r="B34" s="71"/>
+      <c r="C34" s="71"/>
+      <c r="D34" s="66" t="s">
         <v>170</v>
       </c>
       <c r="E34" s="30" t="s">
         <v>171</v>
       </c>
       <c r="F34" s="28"/>
-      <c r="G34" s="68" t="s">
+      <c r="G34" s="58" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="58"/>
-      <c r="B35" s="56"/>
-      <c r="C35" s="56"/>
-      <c r="D35" s="53"/>
+      <c r="A35" s="67"/>
+      <c r="B35" s="71"/>
+      <c r="C35" s="71"/>
+      <c r="D35" s="66"/>
       <c r="E35" s="30" t="s">
         <v>172</v>
       </c>
@@ -2217,10 +2217,10 @@
       </c>
     </row>
     <row r="36" spans="1:7">
-      <c r="A36" s="58"/>
-      <c r="B36" s="56"/>
-      <c r="C36" s="56"/>
-      <c r="D36" s="53"/>
+      <c r="A36" s="67"/>
+      <c r="B36" s="71"/>
+      <c r="C36" s="71"/>
+      <c r="D36" s="66"/>
       <c r="E36" s="30" t="s">
         <v>174</v>
       </c>
@@ -2229,10 +2229,10 @@
       </c>
     </row>
     <row r="37" spans="1:7">
-      <c r="A37" s="58"/>
-      <c r="B37" s="56"/>
-      <c r="C37" s="56"/>
-      <c r="D37" s="53"/>
+      <c r="A37" s="67"/>
+      <c r="B37" s="71"/>
+      <c r="C37" s="71"/>
+      <c r="D37" s="66"/>
       <c r="E37" s="30" t="s">
         <v>173</v>
       </c>
@@ -2241,10 +2241,10 @@
       </c>
     </row>
     <row r="38" spans="1:7">
-      <c r="A38" s="58"/>
-      <c r="B38" s="56"/>
-      <c r="C38" s="56"/>
-      <c r="D38" s="53"/>
+      <c r="A38" s="67"/>
+      <c r="B38" s="71"/>
+      <c r="C38" s="71"/>
+      <c r="D38" s="66"/>
       <c r="E38" s="30" t="s">
         <v>174</v>
       </c>
@@ -2253,10 +2253,10 @@
       </c>
     </row>
     <row r="39" spans="1:7">
-      <c r="A39" s="58"/>
-      <c r="B39" s="56"/>
-      <c r="C39" s="56"/>
-      <c r="D39" s="53"/>
+      <c r="A39" s="67"/>
+      <c r="B39" s="71"/>
+      <c r="C39" s="71"/>
+      <c r="D39" s="66"/>
       <c r="E39" s="30" t="s">
         <v>175</v>
       </c>
@@ -2265,10 +2265,10 @@
       </c>
     </row>
     <row r="40" spans="1:7">
-      <c r="A40" s="58"/>
-      <c r="B40" s="56"/>
-      <c r="C40" s="56"/>
-      <c r="D40" s="59"/>
+      <c r="A40" s="67"/>
+      <c r="B40" s="71"/>
+      <c r="C40" s="71"/>
+      <c r="D40" s="68"/>
       <c r="E40" s="47" t="s">
         <v>176</v>
       </c>
@@ -2277,9 +2277,9 @@
       </c>
     </row>
     <row r="41" spans="1:7">
-      <c r="A41" s="58"/>
-      <c r="B41" s="56"/>
-      <c r="C41" s="56"/>
+      <c r="A41" s="67"/>
+      <c r="B41" s="71"/>
+      <c r="C41" s="71"/>
       <c r="D41" s="31"/>
       <c r="E41" s="30"/>
       <c r="F41" s="40" t="s">
@@ -2287,9 +2287,9 @@
       </c>
     </row>
     <row r="42" spans="1:7">
-      <c r="A42" s="58"/>
-      <c r="B42" s="56"/>
-      <c r="C42" s="56"/>
+      <c r="A42" s="67"/>
+      <c r="B42" s="71"/>
+      <c r="C42" s="71"/>
       <c r="D42" s="31"/>
       <c r="E42" s="30"/>
       <c r="F42" s="40" t="s">
@@ -2297,9 +2297,9 @@
       </c>
     </row>
     <row r="43" spans="1:7">
-      <c r="A43" s="58"/>
-      <c r="B43" s="56"/>
-      <c r="C43" s="56"/>
+      <c r="A43" s="67"/>
+      <c r="B43" s="71"/>
+      <c r="C43" s="71"/>
       <c r="D43" s="49"/>
       <c r="E43" s="49"/>
       <c r="F43" s="40" t="s">
@@ -2307,9 +2307,9 @@
       </c>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="58"/>
-      <c r="B44" s="56"/>
-      <c r="C44" s="53" t="s">
+      <c r="A44" s="67"/>
+      <c r="B44" s="71"/>
+      <c r="C44" s="66" t="s">
         <v>39</v>
       </c>
       <c r="D44" s="31"/>
@@ -2322,9 +2322,9 @@
       </c>
     </row>
     <row r="45" spans="1:7">
-      <c r="A45" s="58"/>
-      <c r="B45" s="56"/>
-      <c r="C45" s="52"/>
+      <c r="A45" s="67"/>
+      <c r="B45" s="71"/>
+      <c r="C45" s="65"/>
       <c r="D45" s="30" t="s">
         <v>144</v>
       </c>
@@ -2334,9 +2334,9 @@
       </c>
     </row>
     <row r="46" spans="1:7">
-      <c r="A46" s="58"/>
-      <c r="B46" s="56"/>
-      <c r="C46" s="52"/>
+      <c r="A46" s="67"/>
+      <c r="B46" s="71"/>
+      <c r="C46" s="65"/>
       <c r="D46" s="30" t="s">
         <v>19</v>
       </c>
@@ -2346,9 +2346,9 @@
       </c>
     </row>
     <row r="47" spans="1:7">
-      <c r="A47" s="58"/>
-      <c r="B47" s="56"/>
-      <c r="C47" s="52"/>
+      <c r="A47" s="67"/>
+      <c r="B47" s="71"/>
+      <c r="C47" s="65"/>
       <c r="D47" s="30" t="s">
         <v>6</v>
       </c>
@@ -2358,9 +2358,9 @@
       </c>
     </row>
     <row r="48" spans="1:7">
-      <c r="A48" s="58"/>
-      <c r="B48" s="56"/>
-      <c r="C48" s="52"/>
+      <c r="A48" s="67"/>
+      <c r="B48" s="71"/>
+      <c r="C48" s="65"/>
       <c r="D48" s="30" t="s">
         <v>74</v>
       </c>
@@ -2370,9 +2370,9 @@
       </c>
     </row>
     <row r="49" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A49" s="58"/>
-      <c r="B49" s="57"/>
-      <c r="C49" s="52"/>
+      <c r="A49" s="67"/>
+      <c r="B49" s="72"/>
+      <c r="C49" s="65"/>
       <c r="D49" s="30" t="s">
         <v>74</v>
       </c>
@@ -2382,7 +2382,7 @@
       </c>
     </row>
     <row r="50" spans="1:7" s="35" customFormat="1" ht="15.75" thickTop="1">
-      <c r="A50" s="52" t="s">
+      <c r="A50" s="65" t="s">
         <v>41</v>
       </c>
       <c r="B50" s="32"/>
@@ -2397,7 +2397,7 @@
       <c r="G50" s="34"/>
     </row>
     <row r="51" spans="1:7">
-      <c r="A51" s="52"/>
+      <c r="A51" s="65"/>
       <c r="B51" s="12"/>
       <c r="C51" s="5"/>
       <c r="D51" s="5" t="s">
@@ -2409,10 +2409,10 @@
       </c>
     </row>
     <row r="52" spans="1:7" ht="30">
-      <c r="A52" s="52"/>
+      <c r="A52" s="65"/>
       <c r="B52" s="12"/>
-      <c r="C52" s="52"/>
-      <c r="D52" s="52" t="s">
+      <c r="C52" s="65"/>
+      <c r="D52" s="65" t="s">
         <v>19</v>
       </c>
       <c r="E52" s="39"/>
@@ -2421,42 +2421,42 @@
       </c>
     </row>
     <row r="53" spans="1:7">
-      <c r="A53" s="52"/>
+      <c r="A53" s="65"/>
       <c r="B53" s="12"/>
-      <c r="C53" s="52"/>
-      <c r="D53" s="52"/>
+      <c r="C53" s="65"/>
+      <c r="D53" s="65"/>
       <c r="E53" s="39"/>
       <c r="F53" s="14" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="45">
-      <c r="A54" s="52"/>
+      <c r="A54" s="65"/>
       <c r="B54" s="12"/>
-      <c r="C54" s="52"/>
-      <c r="D54" s="52"/>
+      <c r="C54" s="65"/>
+      <c r="D54" s="65"/>
       <c r="E54" s="39"/>
       <c r="F54" s="14" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A55" s="52"/>
+      <c r="A55" s="65"/>
       <c r="B55" s="12"/>
-      <c r="C55" s="52"/>
-      <c r="D55" s="52"/>
+      <c r="C55" s="65"/>
+      <c r="D55" s="65"/>
       <c r="E55" s="39"/>
       <c r="F55" s="5" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="56" spans="1:7" s="35" customFormat="1" ht="15.75" thickTop="1">
-      <c r="A56" s="52" t="s">
+      <c r="A56" s="65" t="s">
         <v>47</v>
       </c>
       <c r="B56" s="32"/>
-      <c r="C56" s="52"/>
-      <c r="D56" s="53" t="s">
+      <c r="C56" s="65"/>
+      <c r="D56" s="66" t="s">
         <v>19</v>
       </c>
       <c r="E56" s="40"/>
@@ -2466,47 +2466,47 @@
       <c r="G56" s="34"/>
     </row>
     <row r="57" spans="1:7">
-      <c r="A57" s="52"/>
+      <c r="A57" s="65"/>
       <c r="B57" s="12"/>
-      <c r="C57" s="52"/>
-      <c r="D57" s="52"/>
+      <c r="C57" s="65"/>
+      <c r="D57" s="65"/>
       <c r="E57" s="39"/>
       <c r="F57" s="7" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="30">
-      <c r="A58" s="52"/>
+      <c r="A58" s="65"/>
       <c r="B58" s="12"/>
-      <c r="C58" s="52"/>
-      <c r="D58" s="52"/>
+      <c r="C58" s="65"/>
+      <c r="D58" s="65"/>
       <c r="E58" s="39"/>
       <c r="F58" s="14" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="30">
-      <c r="A59" s="52"/>
+      <c r="A59" s="65"/>
       <c r="B59" s="12"/>
-      <c r="C59" s="52"/>
-      <c r="D59" s="52"/>
+      <c r="C59" s="65"/>
+      <c r="D59" s="65"/>
       <c r="E59" s="39"/>
       <c r="F59" s="14" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="60" spans="1:7">
-      <c r="A60" s="52"/>
+      <c r="A60" s="65"/>
       <c r="B60" s="12"/>
-      <c r="C60" s="52"/>
-      <c r="D60" s="52"/>
+      <c r="C60" s="65"/>
+      <c r="D60" s="65"/>
       <c r="E60" s="39"/>
       <c r="F60" s="5" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A61" s="52"/>
+      <c r="A61" s="65"/>
       <c r="B61" s="12"/>
       <c r="C61" s="5"/>
       <c r="D61" s="5" t="s">
@@ -2518,7 +2518,7 @@
       </c>
     </row>
     <row r="62" spans="1:7" s="35" customFormat="1" ht="15.75" thickTop="1">
-      <c r="A62" s="52" t="s">
+      <c r="A62" s="65" t="s">
         <v>50</v>
       </c>
       <c r="B62" s="32"/>
@@ -2535,9 +2535,9 @@
       <c r="G62" s="34"/>
     </row>
     <row r="63" spans="1:7">
-      <c r="A63" s="52"/>
+      <c r="A63" s="65"/>
       <c r="B63" s="12"/>
-      <c r="C63" s="53" t="s">
+      <c r="C63" s="66" t="s">
         <v>167</v>
       </c>
       <c r="D63" s="5" t="s">
@@ -2549,9 +2549,9 @@
       </c>
     </row>
     <row r="64" spans="1:7">
-      <c r="A64" s="52"/>
+      <c r="A64" s="65"/>
       <c r="B64" s="12"/>
-      <c r="C64" s="52"/>
+      <c r="C64" s="65"/>
       <c r="D64" s="5" t="s">
         <v>54</v>
       </c>
@@ -2561,9 +2561,9 @@
       </c>
     </row>
     <row r="65" spans="1:7">
-      <c r="A65" s="52"/>
+      <c r="A65" s="65"/>
       <c r="B65" s="12"/>
-      <c r="C65" s="52"/>
+      <c r="C65" s="65"/>
       <c r="D65" s="24" t="s">
         <v>168</v>
       </c>
@@ -2573,9 +2573,9 @@
       </c>
     </row>
     <row r="66" spans="1:7">
-      <c r="A66" s="52"/>
+      <c r="A66" s="65"/>
       <c r="B66" s="12"/>
-      <c r="C66" s="52"/>
+      <c r="C66" s="65"/>
       <c r="D66" s="12"/>
       <c r="E66" s="45"/>
       <c r="F66" s="38" t="s">
@@ -2583,9 +2583,9 @@
       </c>
     </row>
     <row r="67" spans="1:7">
-      <c r="A67" s="52"/>
+      <c r="A67" s="65"/>
       <c r="B67" s="12"/>
-      <c r="C67" s="54" t="s">
+      <c r="C67" s="69" t="s">
         <v>166</v>
       </c>
       <c r="D67" s="27" t="s">
@@ -2600,9 +2600,9 @@
       </c>
     </row>
     <row r="68" spans="1:7">
-      <c r="A68" s="52"/>
+      <c r="A68" s="65"/>
       <c r="B68" s="12"/>
-      <c r="C68" s="55"/>
+      <c r="C68" s="70"/>
       <c r="D68" s="27" t="s">
         <v>20</v>
       </c>
@@ -2616,13 +2616,14 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A3:A7"/>
-    <mergeCell ref="C4:C7"/>
-    <mergeCell ref="D4:D7"/>
-    <mergeCell ref="A9:A17"/>
-    <mergeCell ref="C10:C15"/>
-    <mergeCell ref="D10:D15"/>
+    <mergeCell ref="A62:A68"/>
+    <mergeCell ref="C63:C66"/>
+    <mergeCell ref="C67:C68"/>
+    <mergeCell ref="B18:B32"/>
+    <mergeCell ref="A50:A55"/>
+    <mergeCell ref="C52:C55"/>
+    <mergeCell ref="B33:B49"/>
+    <mergeCell ref="C33:C43"/>
     <mergeCell ref="D52:D55"/>
     <mergeCell ref="A56:A61"/>
     <mergeCell ref="C56:C60"/>
@@ -2636,14 +2637,13 @@
     <mergeCell ref="D29:D32"/>
     <mergeCell ref="C44:C49"/>
     <mergeCell ref="D34:D40"/>
-    <mergeCell ref="A62:A68"/>
-    <mergeCell ref="C63:C66"/>
-    <mergeCell ref="C67:C68"/>
-    <mergeCell ref="B18:B32"/>
-    <mergeCell ref="A50:A55"/>
-    <mergeCell ref="C52:C55"/>
-    <mergeCell ref="B33:B49"/>
-    <mergeCell ref="C33:C43"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A3:A7"/>
+    <mergeCell ref="C4:C7"/>
+    <mergeCell ref="D4:D7"/>
+    <mergeCell ref="A9:A17"/>
+    <mergeCell ref="C10:C15"/>
+    <mergeCell ref="D10:D15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -2670,13 +2670,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="63" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
       <c r="F1" s="9"/>
     </row>
     <row r="2" spans="1:6" s="2" customFormat="1" ht="37.5" customHeight="1">
@@ -2711,47 +2711,47 @@
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="53"/>
+      <c r="A4" s="66"/>
       <c r="B4" s="14"/>
-      <c r="C4" s="53"/>
-      <c r="D4" s="53"/>
+      <c r="C4" s="66"/>
+      <c r="D4" s="66"/>
       <c r="E4" s="8" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="53"/>
+      <c r="A5" s="66"/>
       <c r="B5" s="14"/>
-      <c r="C5" s="53"/>
-      <c r="D5" s="53"/>
+      <c r="C5" s="66"/>
+      <c r="D5" s="66"/>
       <c r="E5" s="8" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="53"/>
+      <c r="A6" s="66"/>
       <c r="B6" s="14"/>
-      <c r="C6" s="53"/>
-      <c r="D6" s="53"/>
+      <c r="C6" s="66"/>
+      <c r="D6" s="66"/>
       <c r="E6" s="8" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="53"/>
+      <c r="A7" s="66"/>
       <c r="B7" s="14"/>
-      <c r="C7" s="53"/>
-      <c r="D7" s="53"/>
+      <c r="C7" s="66"/>
+      <c r="D7" s="66"/>
       <c r="E7" s="8" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="53" t="s">
+      <c r="A8" s="66" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="14"/>
-      <c r="C8" s="53" t="s">
+      <c r="C8" s="66" t="s">
         <v>147</v>
       </c>
       <c r="D8" s="30"/>
@@ -2760,9 +2760,9 @@
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="53"/>
+      <c r="A9" s="66"/>
       <c r="B9" s="14"/>
-      <c r="C9" s="53"/>
+      <c r="C9" s="66"/>
       <c r="D9" s="30" t="s">
         <v>18</v>
       </c>
@@ -2771,9 +2771,9 @@
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="53"/>
+      <c r="A10" s="66"/>
       <c r="B10" s="14"/>
-      <c r="C10" s="53"/>
+      <c r="C10" s="66"/>
       <c r="D10" s="30" t="s">
         <v>19</v>
       </c>
@@ -2782,9 +2782,9 @@
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="53"/>
+      <c r="A11" s="66"/>
       <c r="B11" s="14"/>
-      <c r="C11" s="53"/>
+      <c r="C11" s="66"/>
       <c r="D11" s="30" t="s">
         <v>20</v>
       </c>
@@ -2799,7 +2799,7 @@
       <c r="B12" s="11" t="s">
         <v>164</v>
       </c>
-      <c r="C12" s="53" t="s">
+      <c r="C12" s="66" t="s">
         <v>67</v>
       </c>
       <c r="D12" s="30" t="s">
@@ -2810,7 +2810,7 @@
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="C13" s="53"/>
+      <c r="C13" s="66"/>
       <c r="D13" s="30" t="s">
         <v>19</v>
       </c>
@@ -2819,7 +2819,7 @@
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="C14" s="53"/>
+      <c r="C14" s="66"/>
       <c r="D14" s="30" t="s">
         <v>19</v>
       </c>
@@ -2828,7 +2828,7 @@
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="C15" s="53"/>
+      <c r="C15" s="66"/>
       <c r="D15" s="30" t="s">
         <v>19</v>
       </c>
@@ -2837,7 +2837,7 @@
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="C16" s="53"/>
+      <c r="C16" s="66"/>
       <c r="D16" s="30" t="s">
         <v>6</v>
       </c>
@@ -2846,7 +2846,7 @@
       </c>
     </row>
     <row r="17" spans="1:5">
-      <c r="C17" s="53"/>
+      <c r="C17" s="66"/>
       <c r="D17" s="30" t="s">
         <v>19</v>
       </c>
@@ -2867,11 +2867,11 @@
       </c>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="53" t="s">
+      <c r="A19" s="66" t="s">
         <v>68</v>
       </c>
       <c r="B19" s="14"/>
-      <c r="C19" s="53"/>
+      <c r="C19" s="66"/>
       <c r="D19" s="30" t="s">
         <v>43</v>
       </c>
@@ -2880,9 +2880,9 @@
       </c>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="53"/>
+      <c r="A20" s="66"/>
       <c r="B20" s="14"/>
-      <c r="C20" s="53"/>
+      <c r="C20" s="66"/>
       <c r="D20" s="30" t="s">
         <v>6</v>
       </c>
@@ -2891,9 +2891,9 @@
       </c>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="53"/>
+      <c r="A21" s="66"/>
       <c r="B21" s="14"/>
-      <c r="C21" s="53"/>
+      <c r="C21" s="66"/>
       <c r="D21" s="30" t="s">
         <v>19</v>
       </c>
@@ -2902,7 +2902,7 @@
       </c>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="53" t="s">
+      <c r="A22" s="66" t="s">
         <v>69</v>
       </c>
       <c r="B22" s="14"/>
@@ -2915,7 +2915,7 @@
       </c>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="53"/>
+      <c r="A23" s="66"/>
       <c r="B23" s="14"/>
       <c r="C23" s="30"/>
       <c r="D23" s="30" t="s">
@@ -2926,7 +2926,7 @@
       </c>
     </row>
     <row r="24" spans="1:5">
-      <c r="A24" s="53"/>
+      <c r="A24" s="66"/>
       <c r="B24" s="14"/>
       <c r="C24" s="30"/>
       <c r="D24" s="30" t="s">
@@ -2937,7 +2937,7 @@
       </c>
     </row>
     <row r="25" spans="1:5">
-      <c r="A25" s="53"/>
+      <c r="A25" s="66"/>
       <c r="B25" s="14"/>
       <c r="C25" s="30" t="s">
         <v>5</v>
@@ -2950,7 +2950,7 @@
       </c>
     </row>
     <row r="26" spans="1:5">
-      <c r="A26" s="53"/>
+      <c r="A26" s="66"/>
       <c r="B26" s="14"/>
       <c r="C26" s="30"/>
       <c r="D26" s="30" t="s">
@@ -2974,25 +2974,25 @@
       </c>
     </row>
     <row r="28" spans="1:5">
-      <c r="A28" s="53"/>
-      <c r="B28" s="53"/>
-      <c r="C28" s="53"/>
-      <c r="D28" s="53"/>
-      <c r="E28" s="53"/>
+      <c r="A28" s="66"/>
+      <c r="B28" s="66"/>
+      <c r="C28" s="66"/>
+      <c r="D28" s="66"/>
+      <c r="E28" s="66"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A22:A26"/>
+    <mergeCell ref="A28:E28"/>
+    <mergeCell ref="C12:C17"/>
+    <mergeCell ref="A19:A21"/>
+    <mergeCell ref="C19:C21"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A4:A7"/>
     <mergeCell ref="C4:C7"/>
     <mergeCell ref="D4:D7"/>
     <mergeCell ref="A8:A11"/>
     <mergeCell ref="C8:C11"/>
-    <mergeCell ref="A22:A26"/>
-    <mergeCell ref="A28:E28"/>
-    <mergeCell ref="C12:C17"/>
-    <mergeCell ref="A19:A21"/>
-    <mergeCell ref="C19:C21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -3505,15 +3505,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="4.7109375" style="63" customWidth="1"/>
-    <col min="2" max="2" width="41.85546875" style="63" customWidth="1"/>
-    <col min="3" max="3" width="37.85546875" style="63" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" style="63" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="52.5703125" style="63" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="63"/>
+    <col min="1" max="1" width="4.7109375" style="53" customWidth="1"/>
+    <col min="2" max="2" width="41.85546875" style="53" customWidth="1"/>
+    <col min="3" max="3" width="37.85546875" style="53" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" style="53" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="52.5703125" style="53" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="53"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="66" customFormat="1" ht="37.5" customHeight="1">
+    <row r="1" spans="1:5" s="56" customFormat="1" ht="37.5" customHeight="1">
       <c r="A1" s="51" t="s">
         <v>213</v>
       </c>
@@ -3523,10 +3523,10 @@
       <c r="C1" s="51" t="s">
         <v>227</v>
       </c>
-      <c r="D1" s="64" t="s">
+      <c r="D1" s="54" t="s">
         <v>211</v>
       </c>
-      <c r="E1" s="65" t="s">
+      <c r="E1" s="55" t="s">
         <v>212</v>
       </c>
     </row>
@@ -3537,13 +3537,13 @@
       <c r="B2" s="51" t="s">
         <v>215</v>
       </c>
-      <c r="C2" s="67" t="s">
+      <c r="C2" s="57" t="s">
         <v>210</v>
       </c>
-      <c r="D2" s="63" t="s">
+      <c r="D2" s="53" t="s">
         <v>225</v>
       </c>
-      <c r="E2" s="63" t="s">
+      <c r="E2" s="53" t="s">
         <v>229</v>
       </c>
     </row>
@@ -3555,13 +3555,13 @@
       <c r="B3" s="51" t="s">
         <v>216</v>
       </c>
-      <c r="C3" s="67" t="s">
+      <c r="C3" s="57" t="s">
         <v>210</v>
       </c>
-      <c r="D3" s="63" t="s">
+      <c r="D3" s="53" t="s">
         <v>225</v>
       </c>
-      <c r="E3" s="63" t="s">
+      <c r="E3" s="53" t="s">
         <v>230</v>
       </c>
     </row>
@@ -3573,13 +3573,13 @@
       <c r="B4" s="51" t="s">
         <v>217</v>
       </c>
-      <c r="C4" s="67" t="s">
+      <c r="C4" s="57" t="s">
         <v>210</v>
       </c>
-      <c r="D4" s="63" t="s">
+      <c r="D4" s="53" t="s">
         <v>225</v>
       </c>
-      <c r="E4" s="63" t="s">
+      <c r="E4" s="53" t="s">
         <v>231</v>
       </c>
     </row>
@@ -3591,13 +3591,13 @@
       <c r="B5" s="51" t="s">
         <v>224</v>
       </c>
-      <c r="C5" s="67" t="s">
+      <c r="C5" s="57" t="s">
         <v>210</v>
       </c>
-      <c r="D5" s="63" t="s">
+      <c r="D5" s="53" t="s">
         <v>225</v>
       </c>
-      <c r="E5" s="63" t="s">
+      <c r="E5" s="53" t="s">
         <v>232</v>
       </c>
     </row>
@@ -3609,13 +3609,13 @@
       <c r="B6" s="51" t="s">
         <v>218</v>
       </c>
-      <c r="C6" s="67" t="s">
+      <c r="C6" s="57" t="s">
         <v>210</v>
       </c>
-      <c r="D6" s="63" t="s">
+      <c r="D6" s="53" t="s">
         <v>225</v>
       </c>
-      <c r="E6" s="63" t="s">
+      <c r="E6" s="53" t="s">
         <v>233</v>
       </c>
     </row>
@@ -3627,13 +3627,13 @@
       <c r="B7" s="51" t="s">
         <v>219</v>
       </c>
-      <c r="C7" s="67" t="s">
+      <c r="C7" s="57" t="s">
         <v>210</v>
       </c>
-      <c r="D7" s="63" t="s">
+      <c r="D7" s="53" t="s">
         <v>225</v>
       </c>
-      <c r="E7" s="63" t="s">
+      <c r="E7" s="53" t="s">
         <v>234</v>
       </c>
     </row>
@@ -3645,13 +3645,13 @@
       <c r="B8" s="51" t="s">
         <v>214</v>
       </c>
-      <c r="C8" s="67" t="s">
+      <c r="C8" s="57" t="s">
         <v>210</v>
       </c>
-      <c r="D8" s="63" t="s">
+      <c r="D8" s="53" t="s">
         <v>225</v>
       </c>
-      <c r="E8" s="63" t="s">
+      <c r="E8" s="53" t="s">
         <v>235</v>
       </c>
     </row>
@@ -3663,13 +3663,13 @@
       <c r="B9" s="51" t="s">
         <v>220</v>
       </c>
-      <c r="C9" s="67" t="s">
+      <c r="C9" s="57" t="s">
         <v>210</v>
       </c>
-      <c r="D9" s="63" t="s">
+      <c r="D9" s="53" t="s">
         <v>225</v>
       </c>
-      <c r="E9" s="63" t="s">
+      <c r="E9" s="53" t="s">
         <v>236</v>
       </c>
     </row>
@@ -3681,13 +3681,13 @@
       <c r="B10" s="51" t="s">
         <v>221</v>
       </c>
-      <c r="C10" s="67" t="s">
+      <c r="C10" s="57" t="s">
         <v>210</v>
       </c>
-      <c r="D10" s="63" t="s">
+      <c r="D10" s="53" t="s">
         <v>225</v>
       </c>
-      <c r="E10" s="63" t="s">
+      <c r="E10" s="53" t="s">
         <v>237</v>
       </c>
     </row>
@@ -3699,13 +3699,13 @@
       <c r="B11" s="51" t="s">
         <v>222</v>
       </c>
-      <c r="C11" s="67" t="s">
+      <c r="C11" s="57" t="s">
         <v>210</v>
       </c>
-      <c r="D11" s="63" t="s">
+      <c r="D11" s="53" t="s">
         <v>225</v>
       </c>
-      <c r="E11" s="63" t="s">
+      <c r="E11" s="53" t="s">
         <v>238</v>
       </c>
     </row>
@@ -3717,13 +3717,13 @@
       <c r="B12" s="51" t="s">
         <v>223</v>
       </c>
-      <c r="C12" s="67" t="s">
+      <c r="C12" s="57" t="s">
         <v>210</v>
       </c>
-      <c r="D12" s="63" t="s">
+      <c r="D12" s="53" t="s">
         <v>225</v>
       </c>
-      <c r="E12" s="63" t="s">
+      <c r="E12" s="53" t="s">
         <v>239</v>
       </c>
     </row>
@@ -3735,13 +3735,13 @@
       <c r="B13" s="51" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="67" t="s">
+      <c r="C13" s="57" t="s">
         <v>200</v>
       </c>
-      <c r="D13" s="63" t="s">
+      <c r="D13" s="53" t="s">
         <v>226</v>
       </c>
-      <c r="E13" s="63" t="s">
+      <c r="E13" s="53" t="s">
         <v>193</v>
       </c>
     </row>
@@ -3753,13 +3753,13 @@
       <c r="B14" s="51" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="67" t="s">
+      <c r="C14" s="57" t="s">
         <v>200</v>
       </c>
-      <c r="D14" s="63" t="s">
+      <c r="D14" s="53" t="s">
         <v>226</v>
       </c>
-      <c r="E14" s="63" t="s">
+      <c r="E14" s="53" t="s">
         <v>192</v>
       </c>
     </row>
@@ -3771,13 +3771,13 @@
       <c r="B15" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="67" t="s">
+      <c r="C15" s="57" t="s">
         <v>200</v>
       </c>
-      <c r="D15" s="63" t="s">
+      <c r="D15" s="53" t="s">
         <v>226</v>
       </c>
-      <c r="E15" s="63" t="s">
+      <c r="E15" s="53" t="s">
         <v>191</v>
       </c>
     </row>
@@ -3789,13 +3789,13 @@
       <c r="B16" s="51" t="s">
         <v>71</v>
       </c>
-      <c r="C16" s="67" t="s">
+      <c r="C16" s="57" t="s">
         <v>200</v>
       </c>
-      <c r="D16" s="63" t="s">
+      <c r="D16" s="53" t="s">
         <v>226</v>
       </c>
-      <c r="E16" s="63" t="s">
+      <c r="E16" s="53" t="s">
         <v>188</v>
       </c>
     </row>
@@ -3807,13 +3807,13 @@
       <c r="B17" s="51" t="s">
         <v>24</v>
       </c>
-      <c r="C17" s="67" t="s">
+      <c r="C17" s="57" t="s">
         <v>200</v>
       </c>
-      <c r="D17" s="63" t="s">
+      <c r="D17" s="53" t="s">
         <v>226</v>
       </c>
-      <c r="E17" s="63" t="s">
+      <c r="E17" s="53" t="s">
         <v>189</v>
       </c>
     </row>
@@ -3825,13 +3825,13 @@
       <c r="B18" s="51" t="s">
         <v>72</v>
       </c>
-      <c r="C18" s="67" t="s">
+      <c r="C18" s="57" t="s">
         <v>200</v>
       </c>
-      <c r="D18" s="63" t="s">
+      <c r="D18" s="53" t="s">
         <v>226</v>
       </c>
-      <c r="E18" s="63" t="s">
+      <c r="E18" s="53" t="s">
         <v>190</v>
       </c>
     </row>
@@ -3843,13 +3843,13 @@
       <c r="B19" s="51" t="s">
         <v>73</v>
       </c>
-      <c r="C19" s="67" t="s">
+      <c r="C19" s="57" t="s">
         <v>200</v>
       </c>
-      <c r="D19" s="63" t="s">
+      <c r="D19" s="53" t="s">
         <v>226</v>
       </c>
-      <c r="E19" s="63" t="s">
+      <c r="E19" s="53" t="s">
         <v>194</v>
       </c>
     </row>
@@ -3861,13 +3861,13 @@
       <c r="B20" s="51" t="s">
         <v>29</v>
       </c>
-      <c r="C20" s="67" t="s">
+      <c r="C20" s="57" t="s">
         <v>200</v>
       </c>
-      <c r="D20" s="63" t="s">
+      <c r="D20" s="53" t="s">
         <v>226</v>
       </c>
-      <c r="E20" s="63" t="s">
+      <c r="E20" s="53" t="s">
         <v>195</v>
       </c>
     </row>
@@ -3879,13 +3879,13 @@
       <c r="B21" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="C21" s="67" t="s">
+      <c r="C21" s="57" t="s">
         <v>201</v>
       </c>
-      <c r="D21" s="63" t="s">
+      <c r="D21" s="53" t="s">
         <v>226</v>
       </c>
-      <c r="E21" s="63" t="s">
+      <c r="E21" s="53" t="s">
         <v>196</v>
       </c>
     </row>
@@ -3897,13 +3897,13 @@
       <c r="B22" s="51" t="s">
         <v>32</v>
       </c>
-      <c r="C22" s="67" t="s">
+      <c r="C22" s="57" t="s">
         <v>201</v>
       </c>
-      <c r="D22" s="63" t="s">
+      <c r="D22" s="53" t="s">
         <v>226</v>
       </c>
-      <c r="E22" s="63" t="s">
+      <c r="E22" s="53" t="s">
         <v>196</v>
       </c>
     </row>
@@ -3915,13 +3915,13 @@
       <c r="B23" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="C23" s="67" t="s">
+      <c r="C23" s="57" t="s">
         <v>201</v>
       </c>
-      <c r="D23" s="63" t="s">
+      <c r="D23" s="53" t="s">
         <v>226</v>
       </c>
-      <c r="E23" s="63" t="s">
+      <c r="E23" s="53" t="s">
         <v>196</v>
       </c>
     </row>
@@ -3933,13 +3933,13 @@
       <c r="B24" s="51" t="s">
         <v>37</v>
       </c>
-      <c r="C24" s="67" t="s">
+      <c r="C24" s="57" t="s">
         <v>202</v>
       </c>
-      <c r="D24" s="63" t="s">
+      <c r="D24" s="53" t="s">
         <v>226</v>
       </c>
-      <c r="E24" s="63" t="s">
+      <c r="E24" s="53" t="s">
         <v>198</v>
       </c>
     </row>
@@ -3951,13 +3951,13 @@
       <c r="B25" s="51" t="s">
         <v>35</v>
       </c>
-      <c r="C25" s="67" t="s">
+      <c r="C25" s="57" t="s">
         <v>202</v>
       </c>
-      <c r="D25" s="63" t="s">
+      <c r="D25" s="53" t="s">
         <v>226</v>
       </c>
-      <c r="E25" s="63" t="s">
+      <c r="E25" s="53" t="s">
         <v>196</v>
       </c>
     </row>
@@ -3969,13 +3969,13 @@
       <c r="B26" s="51" t="s">
         <v>38</v>
       </c>
-      <c r="C26" s="67" t="s">
+      <c r="C26" s="57" t="s">
         <v>202</v>
       </c>
-      <c r="D26" s="63" t="s">
+      <c r="D26" s="53" t="s">
         <v>226</v>
       </c>
-      <c r="E26" s="63" t="s">
+      <c r="E26" s="53" t="s">
         <v>199</v>
       </c>
     </row>
@@ -3987,13 +3987,13 @@
       <c r="B27" s="51" t="s">
         <v>36</v>
       </c>
-      <c r="C27" s="67" t="s">
+      <c r="C27" s="57" t="s">
         <v>202</v>
       </c>
-      <c r="D27" s="63" t="s">
+      <c r="D27" s="53" t="s">
         <v>226</v>
       </c>
-      <c r="E27" s="63" t="s">
+      <c r="E27" s="53" t="s">
         <v>197</v>
       </c>
     </row>
@@ -4002,16 +4002,16 @@
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="B28" s="63" t="s">
+      <c r="B28" s="53" t="s">
         <v>207</v>
       </c>
-      <c r="C28" s="63" t="s">
+      <c r="C28" s="53" t="s">
         <v>209</v>
       </c>
-      <c r="D28" s="63" t="s">
+      <c r="D28" s="53" t="s">
         <v>225</v>
       </c>
-      <c r="E28" s="63" t="s">
+      <c r="E28" s="53" t="s">
         <v>240</v>
       </c>
     </row>
@@ -4020,16 +4020,16 @@
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="B29" s="63" t="s">
+      <c r="B29" s="53" t="s">
         <v>208</v>
       </c>
-      <c r="C29" s="63" t="s">
+      <c r="C29" s="53" t="s">
         <v>209</v>
       </c>
-      <c r="D29" s="63" t="s">
+      <c r="D29" s="53" t="s">
         <v>225</v>
       </c>
-      <c r="E29" s="63" t="s">
+      <c r="E29" s="53" t="s">
         <v>241</v>
       </c>
     </row>
@@ -4038,16 +4038,16 @@
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="B30" s="63" t="s">
+      <c r="B30" s="53" t="s">
         <v>206</v>
       </c>
-      <c r="C30" s="63" t="s">
+      <c r="C30" s="53" t="s">
         <v>209</v>
       </c>
-      <c r="D30" s="63" t="s">
+      <c r="D30" s="53" t="s">
         <v>225</v>
       </c>
-      <c r="E30" s="63" t="s">
+      <c r="E30" s="53" t="s">
         <v>242</v>
       </c>
     </row>
@@ -4067,144 +4067,144 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="69"/>
-    <col min="2" max="2" width="41.85546875" style="69" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="12" style="69" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" style="69" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="59"/>
+    <col min="2" max="2" width="41.85546875" style="59" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12" style="59" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" style="59" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="59" t="s">
         <v>213</v>
       </c>
-      <c r="B1" s="69" t="s">
+      <c r="B1" s="59" t="s">
         <v>250</v>
       </c>
-      <c r="C1" s="69" t="s">
+      <c r="C1" s="59" t="s">
         <v>251</v>
       </c>
-      <c r="D1" s="69" t="s">
+      <c r="D1" s="59" t="s">
         <v>196</v>
       </c>
-      <c r="E1" s="69" t="s">
+      <c r="E1" s="59" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="69">
+      <c r="A2" s="59">
         <v>0</v>
       </c>
-      <c r="B2" s="69" t="s">
+      <c r="B2" s="59" t="s">
         <v>180</v>
       </c>
-      <c r="C2" s="69">
+      <c r="C2" s="59">
         <v>1945</v>
       </c>
-      <c r="D2" s="69" t="s">
+      <c r="D2" s="59" t="s">
         <v>179</v>
       </c>
-      <c r="E2" s="69" t="s">
+      <c r="E2" s="59" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="69">
+      <c r="A3" s="59">
         <f>SUM(A2+1)</f>
         <v>1</v>
       </c>
-      <c r="B3" s="69" t="s">
+      <c r="B3" s="59" t="s">
         <v>253</v>
       </c>
-      <c r="C3" s="69" t="s">
+      <c r="C3" s="59" t="s">
         <v>247</v>
       </c>
-      <c r="D3" s="69" t="s">
+      <c r="D3" s="59" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="69" t="s">
+      <c r="E3" s="59" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="69">
+      <c r="A4" s="59">
         <f t="shared" ref="A4:A5" si="0">SUM(A3+1)</f>
         <v>2</v>
       </c>
-      <c r="B4" s="69" t="s">
+      <c r="B4" s="59" t="s">
         <v>244</v>
       </c>
-      <c r="C4" s="69" t="s">
+      <c r="C4" s="59" t="s">
         <v>248</v>
       </c>
-      <c r="D4" s="69" t="s">
+      <c r="D4" s="59" t="s">
         <v>33</v>
       </c>
-      <c r="E4" s="69">
+      <c r="E4" s="59">
         <v>2023</v>
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="69">
+      <c r="A5" s="59">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="B5" s="69" t="s">
+      <c r="B5" s="59" t="s">
         <v>246</v>
       </c>
-      <c r="C5" s="69" t="s">
+      <c r="C5" s="59" t="s">
         <v>249</v>
       </c>
-      <c r="D5" s="69" t="s">
+      <c r="D5" s="59" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="69" t="s">
+      <c r="E5" s="59" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="70"/>
-      <c r="D14" s="71"/>
-      <c r="E14" s="70"/>
+      <c r="A14" s="60"/>
+      <c r="D14" s="61"/>
+      <c r="E14" s="60"/>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="70"/>
-      <c r="D15" s="71"/>
-      <c r="E15" s="70"/>
+      <c r="A15" s="60"/>
+      <c r="D15" s="61"/>
+      <c r="E15" s="60"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="70"/>
-      <c r="D16" s="70"/>
-      <c r="E16" s="70"/>
+      <c r="A16" s="60"/>
+      <c r="D16" s="60"/>
+      <c r="E16" s="60"/>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="70"/>
-      <c r="D17" s="71"/>
-      <c r="E17" s="70"/>
+      <c r="A17" s="60"/>
+      <c r="D17" s="61"/>
+      <c r="E17" s="60"/>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="70"/>
-      <c r="D18" s="72"/>
-      <c r="E18" s="70"/>
+      <c r="A18" s="60"/>
+      <c r="D18" s="62"/>
+      <c r="E18" s="60"/>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="70"/>
-      <c r="D19" s="71"/>
-      <c r="E19" s="70"/>
+      <c r="A19" s="60"/>
+      <c r="D19" s="61"/>
+      <c r="E19" s="60"/>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="70"/>
-      <c r="D20" s="71"/>
-      <c r="E20" s="70"/>
+      <c r="A20" s="60"/>
+      <c r="D20" s="61"/>
+      <c r="E20" s="60"/>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="70"/>
-      <c r="D21" s="71"/>
-      <c r="E21" s="70"/>
+      <c r="A21" s="60"/>
+      <c r="D21" s="61"/>
+      <c r="E21" s="60"/>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="70"/>
-      <c r="D22" s="71"/>
-      <c r="E22" s="70"/>
+      <c r="A22" s="60"/>
+      <c r="D22" s="61"/>
+      <c r="E22" s="60"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4226,12 +4226,12 @@
       <c r="A2" t="s">
         <v>203</v>
       </c>
-      <c r="B2" s="62" t="s">
+      <c r="B2" s="52" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="B3" s="62" t="s">
+      <c r="B3" s="52" t="s">
         <v>205</v>
       </c>
     </row>

</xml_diff>